<commit_message>
AUD swap pricer update
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUDSwap.xlsx
+++ b/QuantLibXL/Data2/XLS/AUDSwap.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="105" windowWidth="9600" windowHeight="11175" tabRatio="601" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="15240" windowHeight="8685" tabRatio="601" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Triggers" sheetId="5" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="CapVolsTrigger">Triggers!#REF!</definedName>
     <definedName name="CmsSpreadsTrigger">Triggers!#REF!</definedName>
     <definedName name="Currency">Pricing!$C$1</definedName>
+    <definedName name="Currency2">Pricing!$G$1</definedName>
     <definedName name="Custom" localSheetId="2">FirstLegAdmortization!$F$4:$F$123</definedName>
     <definedName name="Custom" localSheetId="4">SecondLegAdmortization!$F$4:$F$123</definedName>
     <definedName name="Dates" localSheetId="2">FirstLegAdmortization!$B$4:$B$123</definedName>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <t>Notional</t>
   </si>
@@ -282,6 +283,12 @@
   </si>
   <si>
     <t>Business Day Check</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>AudBBSW3M</t>
   </si>
 </sst>
 </file>
@@ -1707,6 +1714,7 @@
       <sheetName val="Swap6M"/>
       <sheetName val="BasisSwap1M3M"/>
       <sheetName val="BasisSwap3M6M"/>
+      <sheetName val="AUD_Market"/>
     </sheetNames>
     <definedNames>
       <definedName name="TriggerCounter" refersTo="='General Settings'!$D$7"/>
@@ -1715,95 +1723,24 @@
       <sheetData sheetId="0">
         <row r="7">
           <cell r="D7">
-            <v>69</v>
+            <v>4</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1">
-        <row r="7">
-          <cell r="D7">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3M</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>AUDOIS3W_Quote</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3W</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>AUDSND_Quote#0000</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>AUD3x6F_Quote</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>Z4</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>V4</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
-      <sheetData sheetId="10">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3AB</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="11">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6AB</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="12">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>3BR</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="13">
-        <row r="7">
-          <cell r="D7" t="str">
-            <v>6BR</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2100,7 +2037,7 @@
   <dimension ref="B1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2125,7 +2062,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="217">
-        <v>41856.418171296296</v>
+        <v>41858.443425925929</v>
       </c>
       <c r="E3" s="213"/>
     </row>
@@ -2136,7 +2073,7 @@
       </c>
       <c r="D4" s="218">
         <f>[1]!TriggerCounter</f>
-        <v>69</v>
+        <v>4</v>
       </c>
       <c r="E4" s="213"/>
     </row>
@@ -2181,7 +2118,7 @@
       </c>
       <c r="D10" s="267">
         <f>IF(D9,_xll.qlSettingsEvaluationDate(Trigger),_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),"1d","f",,Trigger))</f>
-        <v>41856</v>
+        <v>41858</v>
       </c>
       <c r="E10" s="213"/>
     </row>
@@ -2209,7 +2146,7 @@
   <dimension ref="A1:T87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2250,10 +2187,20 @@
       <c r="E1" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="F1" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="65" t="str">
+        <f>UPPER(IF(ISBLANK(F1),H1,F1))</f>
+        <v>AUD</v>
+      </c>
+      <c r="H1" s="11" t="str">
+        <f>I1</f>
+        <v>EUR</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>71</v>
+      </c>
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
       <c r="L1" s="11"/>
@@ -2340,7 +2287,7 @@
       </c>
       <c r="J3" s="103" t="str">
         <f>FirstLegCF</f>
-        <v>obj_00311#0030</v>
+        <v>obj_00951#0019</v>
       </c>
       <c r="K3" s="29" t="b">
         <f>C27</f>
@@ -2348,14 +2295,14 @@
       </c>
       <c r="L3" s="140">
         <f>EvaluationDate</f>
-        <v>41856</v>
+        <v>41858</v>
       </c>
       <c r="M3" s="141">
         <v>0</v>
       </c>
       <c r="N3" s="1" t="str">
         <f>_xll.qlLeg(,M3,L3,,,EvaluationDate)</f>
-        <v>obj_00307#0000</v>
+        <v>obj_00947#0000</v>
       </c>
       <c r="O3" s="1" t="b">
         <v>1</v>
@@ -2373,32 +2320,32 @@
       <c r="B4" s="266"/>
       <c r="C4" s="99">
         <f>IF(ISBLANK(B4),D4,B4)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="D4" s="134">
         <f t="shared" si="1"/>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="E4" s="135">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlInterestRateIndexValueDate(C24,EvaluationDate),"1D","f",,Trigger)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="F4" s="145"/>
       <c r="G4" s="66">
         <f>IF(ISBLANK(F4),H4,F4)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="H4" s="134">
         <f t="shared" ref="H4:H13" si="2">IF(ISBLANK(B4),I4,C4)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="I4" s="135">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlInterestRateIndexValueDate(F24,EvaluationDate),"1D","f",,Trigger)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="J4" s="21" t="str">
         <f>SecondLegCF</f>
-        <v>obj_0030e#0030</v>
+        <v>obj_0094e#0019</v>
       </c>
       <c r="K4" s="27" t="b">
         <f>G27</f>
@@ -2406,14 +2353,14 @@
       </c>
       <c r="L4" s="142">
         <f>_xll.qlCalendarAdvance($C$3,L3,"1D","f")</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="M4" s="143">
         <v>0</v>
       </c>
       <c r="N4" s="1" t="str">
         <f>_xll.qlLeg(,M4,L4,,,EvaluationDate)</f>
-        <v>obj_0030a#0008</v>
+        <v>obj_0094a#0019</v>
       </c>
       <c r="O4" s="1" t="b">
         <f t="shared" ref="O4:O26" si="3">NOT(M4=0)</f>
@@ -2457,21 +2404,21 @@
       </c>
       <c r="J5" s="30" t="str">
         <f>AdditionalCF</f>
-        <v>obj_00310#0023</v>
+        <v>obj_00950#0019</v>
       </c>
       <c r="K5" s="30" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="142">
         <f>_xll.qlCalendarAdvance($C$3,L4,"1D","f")</f>
-        <v>41858</v>
+        <v>41862</v>
       </c>
       <c r="M5" s="143">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="str">
         <f>_xll.qlLeg(,M5,L5,,,EvaluationDate)</f>
-        <v>obj_00309#0008</v>
+        <v>obj_00949#0019</v>
       </c>
       <c r="O5" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2517,14 +2464,14 @@
       <c r="K6" s="5"/>
       <c r="L6" s="142">
         <f>_xll.qlCalendarAdvance($C$3,L5,"1D","f")</f>
-        <v>41859</v>
+        <v>41863</v>
       </c>
       <c r="M6" s="143">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="str">
         <f>_xll.qlLeg(,M6,L6,,,EvaluationDate)</f>
-        <v>obj_0030b#0008</v>
+        <v>obj_0094b#0019</v>
       </c>
       <c r="O6" s="1" t="b">
         <f t="shared" si="3"/>
@@ -2593,28 +2540,28 @@
       <c r="B8" s="4"/>
       <c r="C8" s="99">
         <f t="shared" si="0"/>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="D8" s="134">
         <f t="shared" si="1"/>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="E8" s="135">
         <f>_xll.qlCalendarAdvance("NULLCALENDAR",C$4,C$7,"Unadjusted")</f>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="F8" s="145"/>
       <c r="G8" s="66">
         <f t="shared" si="4"/>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="H8" s="134">
         <f t="shared" si="2"/>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="I8" s="135">
         <f>_xll.qlCalendarAdvance("NULLCALENDAR",G$4,G$7,"Unadjusted")</f>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -2889,21 +2836,21 @@
       <c r="B14" s="17"/>
       <c r="C14" s="102" t="str">
         <f t="shared" si="0"/>
-        <v>obj_0030d#0028</v>
+        <v>obj_0094d#0019</v>
       </c>
       <c r="D14" s="138" t="str">
         <f>_xll.qlSchedule(,C4,C8,C9,C3,C10,C11,C12,C13,C5,C6)</f>
-        <v>obj_0030d#0028</v>
+        <v>obj_0094d#0019</v>
       </c>
       <c r="E14" s="139"/>
       <c r="F14" s="115"/>
       <c r="G14" s="70" t="str">
         <f>IF(ISBLANK(F14),H14,F14)</f>
-        <v>obj_0030c#0028</v>
+        <v>obj_0094c#0019</v>
       </c>
       <c r="H14" s="138" t="str">
         <f>_xll.qlSchedule(,G4,G8,G9,G3,G10,G11,G12,G13,G5,G6)</f>
-        <v>obj_0030c#0028</v>
+        <v>obj_0094c#0019</v>
       </c>
       <c r="I14" s="139"/>
       <c r="J14" s="5"/>
@@ -3353,18 +3300,18 @@
         <v>4</v>
       </c>
       <c r="B24" s="113" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C24" s="98" t="str">
         <f t="shared" si="5"/>
-        <v>AudBBSW6M</v>
+        <v>AudBBSW3M</v>
       </c>
       <c r="D24" s="127" t="str">
         <f t="shared" si="7"/>
         <v>AudBBSW6M</v>
       </c>
       <c r="E24" s="128" t="str">
-        <f>PROPER(Currency)&amp;"BBSW"&amp;"6M"</f>
+        <f>PROPER(Currency)&amp;IF(Currency="AUD","BBSW","ibor")&amp;"6M"</f>
         <v>AudBBSW6M</v>
       </c>
       <c r="F24" s="113" t="s">
@@ -3532,14 +3479,14 @@
       <c r="K27" s="5"/>
       <c r="L27" s="142">
         <f>_xll.qlCalendarAdjust($C$3,E8,$C$11)</f>
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="M27" s="143">
         <v>0</v>
       </c>
       <c r="N27" s="1" t="str">
         <f>_xll.qlLeg(,M27,L27,,,EvaluationDate)</f>
-        <v>obj_0030f#0023</v>
+        <v>obj_0094f#0019</v>
       </c>
       <c r="O27" s="1" t="b">
         <v>1</v>
@@ -3557,21 +3504,21 @@
       <c r="B28" s="105"/>
       <c r="C28" s="106" t="str">
         <f>IF(ISBLANK(B28),D28,B28)</f>
-        <v>obj_00311#0030</v>
+        <v>obj_00951#0019</v>
       </c>
       <c r="D28" s="130" t="str">
         <f>_xll.qlIborLeg(B28,C16,_xll.ohPack(FirstLegAdmortization!Effective),C14,C19,C20,C21,C22,C23,C24,C25,C26)</f>
-        <v>obj_00311#0030</v>
+        <v>obj_00951#0019</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="115"/>
       <c r="G28" s="75" t="str">
         <f t="shared" si="6"/>
-        <v>obj_0030e#0030</v>
+        <v>obj_0094e#0019</v>
       </c>
       <c r="H28" s="130" t="str">
         <f>_xll.qlIborLeg(F28,G16,_xll.ohPack(SecondLegAdmortization!Effective),G14,G19,G20,G21,G22,G23,G24,G25,G26)</f>
-        <v>obj_0030e#0030</v>
+        <v>obj_0094e#0019</v>
       </c>
       <c r="I28" s="15"/>
       <c r="J28" s="5"/>
@@ -3579,11 +3526,11 @@
       <c r="L28" s="144"/>
       <c r="M28" s="65" t="str">
         <f>IF(ISBLANK(L28),N28,L28)</f>
-        <v>obj_00310#0023</v>
+        <v>obj_00950#0019</v>
       </c>
       <c r="N28" s="26" t="str">
         <f>_xll.qlMultiPhaseLeg(,_xll.ohFilter(N3:N27,O3:O27),FALSE)</f>
-        <v>obj_00310#0023</v>
+        <v>obj_00950#0019</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3599,7 +3546,7 @@
       <c r="B29" s="132"/>
       <c r="C29" s="19" t="str">
         <f>_xll.qlSwap(B29,$J$3:$J$5,$K$3:$K$5)</f>
-        <v>obj_00312#0030</v>
+        <v>obj_00952#0019</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="9"/>
@@ -3648,15 +3595,15 @@
       <c r="B31" s="18"/>
       <c r="C31" s="92" t="str">
         <f>IF(ISBLANK(B31),D31,IF(ISNUMBER(B31),_xll.qlConstantOptionletVol(,_xll.qlSimpleQuote(,B31),C3),B31))</f>
-        <v>Aud6MCapletVol</v>
+        <v>Aud3MCapletVol</v>
       </c>
       <c r="D31" s="115" t="str">
         <f>E31</f>
-        <v>Aud6MCapletVol</v>
+        <v>Aud3MCapletVol</v>
       </c>
       <c r="E31" s="115" t="str">
         <f>PROPER(Currency)&amp;_xll.qlInterestRateIndexTenor(C24)&amp;"CapletVol"</f>
-        <v>Aud6MCapletVol</v>
+        <v>Aud3MCapletVol</v>
       </c>
       <c r="F31" s="18"/>
       <c r="G31" s="19" t="str">
@@ -3851,7 +3798,9 @@
       <c r="A37" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B37" s="81"/>
+      <c r="B37" s="81" t="s">
+        <v>68</v>
+      </c>
       <c r="C37" s="19" t="str">
         <f>IF(ISBLANK(B37),D37, IF(ISNUMBER(B37),_xll.qlFlatForward(,0,"NullCalendar",B37,,"continuous","annual"),B37))</f>
         <v>AUDON</v>
@@ -3934,11 +3883,11 @@
       <c r="B40" s="28"/>
       <c r="C40" s="167">
         <f>IF(ISBLANK(B40),D40,B40)</f>
-        <v>41856</v>
+        <v>41858</v>
       </c>
       <c r="D40" s="148">
         <f>EvaluationDate</f>
-        <v>41856</v>
+        <v>41858</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -3964,11 +3913,11 @@
       <c r="B41" s="28"/>
       <c r="C41" s="167">
         <f>IF(ISBLANK(B41),D41,B41)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="D41" s="148">
         <f>E4</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -3994,11 +3943,11 @@
       <c r="B42" s="151"/>
       <c r="C42" s="74" t="str">
         <f>IF(ISBLANK(B42),D42,B42)</f>
-        <v>obj_00308#0000</v>
+        <v>obj_00948#0030</v>
       </c>
       <c r="D42" s="149" t="str">
         <f>_xll.qlDiscountingSwapEngine(,DiscountCurve,IncludeSettlementDate,SettlementDate,NPVDate)</f>
-        <v>obj_00308#0000</v>
+        <v>obj_00948#0030</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -4073,7 +4022,7 @@
       <c r="B45" s="83"/>
       <c r="C45" s="84">
         <f>_xll.ohTrigger(AllTriggers,C43,ISERROR(C35),ISERROR(G35))</f>
-        <v>86</v>
+        <v>39</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
@@ -4122,7 +4071,7 @@
       <c r="B47" s="85"/>
       <c r="C47" s="86">
         <f>_xll.qlInstrumentNPV(SwapID,C45)</f>
-        <v>327636.71811145375</v>
+        <v>326659.31446070294</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -4171,14 +4120,14 @@
       <c r="B49" s="152"/>
       <c r="C49" s="153">
         <f>C$25-NPV/C$51/10000</f>
-        <v>3.8525000000093658E-2</v>
+        <v>3.834999999999749E-2</v>
       </c>
       <c r="D49" s="156"/>
       <c r="E49" s="156"/>
       <c r="F49" s="152"/>
       <c r="G49" s="153">
         <f>G$25-NPV/G$51/10000</f>
-        <v>-3.8525000000093658E-2</v>
+        <v>-3.834999999999749E-2</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -4208,7 +4157,7 @@
       <c r="F50" s="92"/>
       <c r="G50" s="157">
         <f>_xll.qlSwapLegNPV(SwapID,1,$C$45)</f>
-        <v>327636.71811145375</v>
+        <v>326659.31446070294</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -4234,14 +4183,14 @@
       <c r="B51" s="152"/>
       <c r="C51" s="159">
         <f>_xll.qlSwapLegBPS(SwapID,0,C45)</f>
-        <v>-850.45222092318556</v>
+        <v>-851.78439233565655</v>
       </c>
       <c r="D51" s="156"/>
       <c r="E51" s="156"/>
       <c r="F51" s="152"/>
       <c r="G51" s="159">
         <f>_xll.qlSwapLegBPS(SwapID,1,C45)</f>
-        <v>850.45222092318556</v>
+        <v>851.78439233565655</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
@@ -5019,14 +4968,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18 I18 E18:F18">
       <formula1>"None,Custom,Step,French"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24">
-      <formula1>"AudBBSW3M,AudBBSW6M"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 F1 I1">
       <formula1>"EUR,USD,GBP,JPY,CHF,AUD,CNY,CNH,HKD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24">
-      <formula1>"AudBBSW3M,AudBBSW6M"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 F24">
+      <formula1>"AudBBSW3M,AudBBSW6M,Euribor3M,Euribor6M"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
+      <formula1>"AUDON,AUDSTD,AUDEURBASOIS,AUDEURBASSTD"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5060,7 +5009,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="35" t="str">
         <f>Pricing!$C$14</f>
-        <v>obj_0030d#0028</v>
+        <v>obj_0094d#0019</v>
       </c>
       <c r="C1" s="34" t="str">
         <f>UPPER(Pricing!$C$18)</f>
@@ -5117,7 +5066,7 @@
       </c>
       <c r="B4" s="42">
         <f t="array" ref="B4:B123">_xll.qlScheduleDates(Schedule)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="C4" s="44">
         <f t="array" ref="C4:C123">IF(Type="MIRROR",E4:E123,IF(Type="CUSTOM",F4:F123,IF(Type="STEP",G4:G123,IF(Type="FRENCH",H4:H123,D4:D123))))</f>
@@ -5153,7 +5102,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="42">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="C5" s="44">
         <v>1000000</v>
@@ -5187,7 +5136,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="42">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="C6" s="44">
         <v>1000000</v>
@@ -5289,7 +5238,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="42">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="C9" s="44">
         <v>1000000</v>
@@ -5357,7 +5306,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="42">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="C11" s="44">
         <v>1000000</v>
@@ -5391,7 +5340,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="42">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="C12" s="44">
         <v>1000000</v>
@@ -5425,7 +5374,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="42">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="C13" s="44">
         <v>1000000</v>
@@ -5459,7 +5408,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="42">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="C14" s="44">
         <v>1000000</v>
@@ -5493,7 +5442,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="42">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="C15" s="44">
         <v>1000000</v>
@@ -5527,7 +5476,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="42">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="C16" s="44">
         <v>1000000</v>
@@ -5595,7 +5544,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="42">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="C18" s="44">
         <v>1000000</v>
@@ -5629,7 +5578,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="42">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="C19" s="44">
         <v>1000000</v>
@@ -5697,7 +5646,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="42">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="C21" s="44">
         <v>1000000</v>
@@ -5765,7 +5714,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="42">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="C23" s="44">
         <v>1000000</v>
@@ -5799,7 +5748,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="42">
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="C24" s="44" t="e">
         <v>#N/A</v>
@@ -9322,10 +9271,10 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="186">
         <f t="array" ref="A3:A122">_xll.qlYieldTSDiscount(DiscountCurve,_xll.ohPack(B3:B122))</f>
-        <v>0.98754793665072238</v>
+        <v>0.98762977471753821</v>
       </c>
       <c r="B3" s="187">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="C3" s="188">
         <v>0</v>
@@ -9334,13 +9283,13 @@
         <v>1000000</v>
       </c>
       <c r="E3" s="187">
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="F3" s="187">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="G3" s="189">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H3" s="190" t="str">
         <v>#N/A</v>
@@ -9355,7 +9304,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L3" s="192">
-        <v>0.50410958904109593</v>
+        <v>0.50684931506849318</v>
       </c>
       <c r="M3" s="193">
         <v>0</v>
@@ -9387,10 +9336,10 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="196">
-        <v>0.97559053340586988</v>
+        <v>0.97593905629035904</v>
       </c>
       <c r="B4" s="175">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="C4" s="177">
         <v>0</v>
@@ -9399,13 +9348,13 @@
         <v>1000000</v>
       </c>
       <c r="E4" s="175">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="F4" s="175">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="G4" s="176">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H4" s="178" t="str">
         <v>#N/A</v>
@@ -9420,7 +9369,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L4" s="180">
-        <v>0.49589041095890413</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M4" s="181">
         <v>0</v>
@@ -9452,7 +9401,7 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="196">
-        <v>0.96283561957237329</v>
+        <v>0.963823130511412</v>
       </c>
       <c r="B5" s="175">
         <v>42408</v>
@@ -9464,13 +9413,13 @@
         <v>1000000</v>
       </c>
       <c r="E5" s="175">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="F5" s="175">
         <v>42408</v>
       </c>
       <c r="G5" s="176">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H5" s="178" t="str">
         <v>#N/A</v>
@@ -9485,7 +9434,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L5" s="180">
-        <v>0.50958904109589043</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M5" s="181">
         <v>0</v>
@@ -9517,7 +9466,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="196">
-        <v>0.94967175418405925</v>
+        <v>0.95091964847149946</v>
       </c>
       <c r="B6" s="175">
         <v>42590</v>
@@ -9582,10 +9531,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="196">
-        <v>0.93583359827214774</v>
+        <v>0.9372080274699961</v>
       </c>
       <c r="B7" s="175">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="C7" s="177">
         <v>0</v>
@@ -9597,10 +9546,10 @@
         <v>42590</v>
       </c>
       <c r="F7" s="175">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="G7" s="176">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H7" s="178" t="str">
         <v>#N/A</v>
@@ -9615,7 +9564,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L7" s="180">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M7" s="181">
         <v>0</v>
@@ -9647,7 +9596,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="196">
-        <v>0.92143275179637318</v>
+        <v>0.92319139827288144</v>
       </c>
       <c r="B8" s="175">
         <v>42955</v>
@@ -9659,13 +9608,13 @@
         <v>1000000</v>
       </c>
       <c r="E8" s="175">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="F8" s="175">
         <v>42955</v>
       </c>
       <c r="G8" s="176">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H8" s="178" t="str">
         <v>#N/A</v>
@@ -9680,7 +9629,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L8" s="180">
-        <v>0.50136986301369868</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M8" s="181">
         <v>0</v>
@@ -9712,10 +9661,10 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="196">
-        <v>0.90679493634089159</v>
+        <v>0.90848563416936845</v>
       </c>
       <c r="B9" s="175">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="C9" s="177">
         <v>0</v>
@@ -9727,10 +9676,10 @@
         <v>42955</v>
       </c>
       <c r="F9" s="175">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="G9" s="176">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H9" s="178" t="str">
         <v>#N/A</v>
@@ -9745,7 +9694,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L9" s="180">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M9" s="181">
         <v>0</v>
@@ -9777,10 +9726,10 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="196">
-        <v>0.89180866948193593</v>
+        <v>0.89360865189861183</v>
       </c>
       <c r="B10" s="175">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="C10" s="177">
         <v>0</v>
@@ -9789,13 +9738,13 @@
         <v>1000000</v>
       </c>
       <c r="E10" s="175">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="F10" s="175">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="G10" s="176">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H10" s="178" t="str">
         <v>#N/A</v>
@@ -9810,7 +9759,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L10" s="180">
-        <v>0.49863013698630138</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M10" s="181">
         <v>0</v>
@@ -9842,10 +9791,10 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="196">
-        <v>0.87635138893012232</v>
+        <v>0.87810972118544339</v>
       </c>
       <c r="B11" s="175">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="C11" s="177">
         <v>0</v>
@@ -9854,13 +9803,13 @@
         <v>1000000</v>
       </c>
       <c r="E11" s="175">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="F11" s="175">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="G11" s="176">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H11" s="178" t="str">
         <v>#N/A</v>
@@ -9875,7 +9824,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L11" s="180">
-        <v>0.50136986301369868</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M11" s="181">
         <v>0</v>
@@ -9907,10 +9856,10 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="196">
-        <v>0.86080364957416167</v>
+        <v>0.86258376609713372</v>
       </c>
       <c r="B12" s="175">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="C12" s="177">
         <v>0</v>
@@ -9919,10 +9868,10 @@
         <v>1000000</v>
       </c>
       <c r="E12" s="175">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="F12" s="175">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="G12" s="176">
         <v>181</v>
@@ -9972,10 +9921,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="196">
-        <v>0.84481831838569088</v>
+        <v>0.84638478006872575</v>
       </c>
       <c r="B13" s="175">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="C13" s="177">
         <v>0</v>
@@ -9984,13 +9933,13 @@
         <v>1000000</v>
       </c>
       <c r="E13" s="175">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="F13" s="175">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="G13" s="176">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H13" s="178" t="str">
         <v>#N/A</v>
@@ -10005,7 +9954,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L13" s="180">
-        <v>0.50410958904109593</v>
+        <v>0.50958904109589043</v>
       </c>
       <c r="M13" s="181">
         <v>0</v>
@@ -10037,10 +9986,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="196">
-        <v>0.82862259521329318</v>
+        <v>0.83012725902555851</v>
       </c>
       <c r="B14" s="175">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="C14" s="177">
         <v>0</v>
@@ -10049,10 +9998,10 @@
         <v>1000000</v>
       </c>
       <c r="E14" s="175">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="F14" s="175">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="G14" s="176">
         <v>182</v>
@@ -10102,7 +10051,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="196">
-        <v>0.81160713553623487</v>
+        <v>0.8134325054127004</v>
       </c>
       <c r="B15" s="175">
         <v>44235</v>
@@ -10114,13 +10063,13 @@
         <v>1000000</v>
       </c>
       <c r="E15" s="175">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="F15" s="175">
         <v>44235</v>
       </c>
       <c r="G15" s="176">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H15" s="178" t="str">
         <v>#N/A</v>
@@ -10135,7 +10084,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L15" s="180">
-        <v>0.50958904109589043</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M15" s="181">
         <v>0</v>
@@ -10167,10 +10116,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="196">
-        <v>0.79544497159972916</v>
+        <v>0.79692238577986874</v>
       </c>
       <c r="B16" s="175">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="C16" s="177">
         <v>0</v>
@@ -10182,10 +10131,10 @@
         <v>44235</v>
       </c>
       <c r="F16" s="175">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="G16" s="176">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H16" s="178" t="str">
         <v>#N/A</v>
@@ -10200,7 +10149,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L16" s="180">
-        <v>0.49041095890410957</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M16" s="181">
         <v>0</v>
@@ -10232,10 +10181,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="196">
-        <v>0.77951065610534276</v>
+        <v>0.78102890658709501</v>
       </c>
       <c r="B17" s="175">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="C17" s="177">
         <v>0</v>
@@ -10244,13 +10193,13 @@
         <v>1000000</v>
       </c>
       <c r="E17" s="175">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="F17" s="175">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="G17" s="176">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H17" s="178" t="str">
         <v>#N/A</v>
@@ -10265,7 +10214,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L17" s="180">
-        <v>0.50684931506849318</v>
+        <v>0.50136986301369868</v>
       </c>
       <c r="M17" s="181">
         <v>0</v>
@@ -10297,7 +10246,7 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="196">
-        <v>0.76413364028636954</v>
+        <v>0.76564045846940665</v>
       </c>
       <c r="B18" s="175">
         <v>44781</v>
@@ -10309,13 +10258,13 @@
         <v>1000000</v>
       </c>
       <c r="E18" s="175">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="F18" s="175">
         <v>44781</v>
       </c>
       <c r="G18" s="176">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H18" s="178" t="str">
         <v>#N/A</v>
@@ -10330,7 +10279,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L18" s="180">
-        <v>0.49863013698630138</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M18" s="181">
         <v>0</v>
@@ -10362,10 +10311,10 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="196">
-        <v>0.74852864113593476</v>
+        <v>0.74986498717119976</v>
       </c>
       <c r="B19" s="175">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="C19" s="177">
         <v>0</v>
@@ -10377,10 +10326,10 @@
         <v>44781</v>
       </c>
       <c r="F19" s="175">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="G19" s="176">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H19" s="178" t="str">
         <v>#N/A</v>
@@ -10395,7 +10344,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L19" s="180">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M19" s="181">
         <v>0</v>
@@ -10427,7 +10376,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="196">
-        <v>0.7326415617948786</v>
+        <v>0.73411965313311145</v>
       </c>
       <c r="B20" s="175">
         <v>45146</v>
@@ -10439,13 +10388,13 @@
         <v>1000000</v>
       </c>
       <c r="E20" s="175">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="F20" s="175">
         <v>45146</v>
       </c>
       <c r="G20" s="176">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H20" s="178" t="str">
         <v>#N/A</v>
@@ -10460,7 +10409,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L20" s="180">
-        <v>0.50136986301369868</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M20" s="181">
         <v>0</v>
@@ -10492,10 +10441,10 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="196">
-        <v>0.71681099301552698</v>
+        <v>0.71794182972811249</v>
       </c>
       <c r="B21" s="175">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="C21" s="177">
         <v>0</v>
@@ -10507,10 +10456,10 @@
         <v>45146</v>
       </c>
       <c r="F21" s="175">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="G21" s="176">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H21" s="178" t="str">
         <v>#N/A</v>
@@ -10525,7 +10474,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L21" s="180">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M21" s="181">
         <v>0</v>
@@ -10557,10 +10506,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="196">
-        <v>0.70112984314388349</v>
+        <v>0.70208555969117814</v>
       </c>
       <c r="B22" s="175">
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="C22" s="177">
         <v>0</v>
@@ -10569,10 +10518,10 @@
         <v>1000000</v>
       </c>
       <c r="E22" s="175">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="F22" s="175">
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="G22" s="176">
         <v>182</v>
@@ -17153,7 +17102,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="35" t="str">
         <f>Pricing!$G$14</f>
-        <v>obj_0030c#0028</v>
+        <v>obj_0094c#0019</v>
       </c>
       <c r="C1" s="34" t="str">
         <f>UPPER(Pricing!$G$18)</f>
@@ -17210,7 +17159,7 @@
       </c>
       <c r="B4" s="42">
         <f t="array" ref="B4:B123">_xll.qlScheduleDates(Schedule)</f>
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="C4" s="44">
         <f t="array" ref="C4:C123">IF(Type="MIRROR",E4:E123,IF(Type="CUSTOM",F4:F123,IF(Type="STEP",G4:G123,IF(Type="FRENCH",H4:H123,D4:D123))))</f>
@@ -17246,7 +17195,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="42">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="C5" s="44">
         <v>1000000</v>
@@ -17280,7 +17229,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="42">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="C6" s="44">
         <v>1000000</v>
@@ -17382,7 +17331,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="42">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="C9" s="44">
         <v>1000000</v>
@@ -17450,7 +17399,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="42">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="C11" s="44">
         <v>1000000</v>
@@ -17484,7 +17433,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="42">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="C12" s="44">
         <v>1000000</v>
@@ -17518,7 +17467,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="42">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="C13" s="44">
         <v>1000000</v>
@@ -17552,7 +17501,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="42">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="C14" s="44">
         <v>1000000</v>
@@ -17586,7 +17535,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="42">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="C15" s="44">
         <v>1000000</v>
@@ -17620,7 +17569,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="42">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="C16" s="44">
         <v>1000000</v>
@@ -17688,7 +17637,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="42">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="C18" s="44">
         <v>1000000</v>
@@ -17722,7 +17671,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="42">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="C19" s="44">
         <v>1000000</v>
@@ -17790,7 +17739,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="42">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="C21" s="44">
         <v>1000000</v>
@@ -17858,7 +17807,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="42">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="C23" s="44">
         <v>1000000</v>
@@ -17892,7 +17841,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="42">
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="C24" s="44" t="e">
         <v>#N/A</v>
@@ -21420,25 +21369,25 @@
     <row r="3" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="225">
         <f t="array" ref="A3:A122">_xll.qlYieldTSDiscount(DiscountCurve,_xll.ohPack(B3:B122))</f>
-        <v>0.98754793665072238</v>
+        <v>0.98762977471753821</v>
       </c>
       <c r="B3" s="226">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="C3" s="227">
-        <v>13734.319065914267</v>
+        <v>13809.438866008386</v>
       </c>
       <c r="D3" s="227">
         <v>1000000</v>
       </c>
       <c r="E3" s="226">
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="F3" s="226">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="G3" s="228">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H3" s="229" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21447,16 +21396,16 @@
         <v>0</v>
       </c>
       <c r="J3" s="226">
-        <v>41857</v>
+        <v>41859</v>
       </c>
       <c r="K3" s="228" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L3" s="231">
-        <v>0.50410958904109593</v>
+        <v>0.50684931506849318</v>
       </c>
       <c r="M3" s="232">
-        <v>2.724470901662341E-2</v>
+        <v>2.7245649654557082E-2</v>
       </c>
       <c r="N3" s="232" t="str">
         <v>#N/A</v>
@@ -21465,10 +21414,10 @@
         <v>1</v>
       </c>
       <c r="P3" s="232">
-        <v>2.7244709016623413E-2</v>
+        <v>2.7245649654557079E-2</v>
       </c>
       <c r="Q3" s="232">
-        <v>-3.4694469519536142E-18</v>
+        <v>3.4694469519536142E-18</v>
       </c>
       <c r="R3" s="232">
         <v>0</v>
@@ -21504,25 +21453,25 @@
     </row>
     <row r="4" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="237">
-        <v>0.97559053340586988</v>
+        <v>0.97593905629035904</v>
       </c>
       <c r="B4" s="238">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="C4" s="239">
-        <v>13100.494964233712</v>
+        <v>12656.249528957942</v>
       </c>
       <c r="D4" s="239">
         <v>1000000</v>
       </c>
       <c r="E4" s="238">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="F4" s="238">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="G4" s="240">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H4" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21531,16 +21480,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="238">
-        <v>42041</v>
+        <v>42044</v>
       </c>
       <c r="K4" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L4" s="243">
-        <v>0.49589041095890413</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M4" s="244">
-        <v>2.6418125204117706E-2</v>
+        <v>2.5382038890492575E-2</v>
       </c>
       <c r="N4" s="244" t="str">
         <v>#N/A</v>
@@ -21549,10 +21498,10 @@
         <v>1</v>
       </c>
       <c r="P4" s="244">
-        <v>2.6418125204117703E-2</v>
+        <v>2.5382038890492575E-2</v>
       </c>
       <c r="Q4" s="244">
-        <v>3.4694469519536142E-18</v>
+        <v>0</v>
       </c>
       <c r="R4" s="244">
         <v>0</v>
@@ -21588,25 +21537,25 @@
     </row>
     <row r="5" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="237">
-        <v>0.96283561957237329</v>
+        <v>0.963823130511412</v>
       </c>
       <c r="B5" s="238">
         <v>42408</v>
       </c>
       <c r="C5" s="239">
-        <v>14432.607618412474</v>
+        <v>13717.233720262899</v>
       </c>
       <c r="D5" s="239">
         <v>1000000</v>
       </c>
       <c r="E5" s="238">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="F5" s="238">
         <v>42408</v>
       </c>
       <c r="G5" s="240">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H5" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21615,16 +21564,16 @@
         <v>0</v>
       </c>
       <c r="J5" s="238">
-        <v>42222</v>
+        <v>42226</v>
       </c>
       <c r="K5" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L5" s="243">
-        <v>0.50958904109589043</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M5" s="244">
-        <v>2.83220525845191E-2</v>
+        <v>2.7509836856571199E-2</v>
       </c>
       <c r="N5" s="244" t="str">
         <v>#N/A</v>
@@ -21633,10 +21582,10 @@
         <v>1</v>
       </c>
       <c r="P5" s="244">
-        <v>2.83220525845191E-2</v>
+        <v>2.7509836856571202E-2</v>
       </c>
       <c r="Q5" s="244">
-        <v>0</v>
+        <v>-3.4694469519536142E-18</v>
       </c>
       <c r="R5" s="244">
         <v>0</v>
@@ -21672,13 +21621,13 @@
     </row>
     <row r="6" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="237">
-        <v>0.94967175418405925</v>
+        <v>0.95091964847149946</v>
       </c>
       <c r="B6" s="238">
         <v>42590</v>
       </c>
       <c r="C6" s="239">
-        <v>15228.701785811705</v>
+        <v>14974.502738472895</v>
       </c>
       <c r="D6" s="239">
         <v>1000000</v>
@@ -21708,7 +21657,7 @@
         <v>0.49863013698630138</v>
       </c>
       <c r="M6" s="244">
-        <v>3.0541077757259737E-2</v>
+        <v>3.0031282964519814E-2</v>
       </c>
       <c r="N6" s="244" t="str">
         <v>#N/A</v>
@@ -21717,7 +21666,7 @@
         <v>1</v>
       </c>
       <c r="P6" s="244">
-        <v>3.0541077757259737E-2</v>
+        <v>3.0031282964519814E-2</v>
       </c>
       <c r="Q6" s="244">
         <v>0</v>
@@ -21756,13 +21705,13 @@
     </row>
     <row r="7" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="237">
-        <v>0.93583359827214774</v>
+        <v>0.9372080274699961</v>
       </c>
       <c r="B7" s="238">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="C7" s="239">
-        <v>16120.487722126598</v>
+        <v>16043.609291996885</v>
       </c>
       <c r="D7" s="239">
         <v>1000000</v>
@@ -21771,10 +21720,10 @@
         <v>42590</v>
       </c>
       <c r="F7" s="238">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="G7" s="240">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H7" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21789,10 +21738,10 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L7" s="243">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M7" s="244">
-        <v>3.2329549552616528E-2</v>
+        <v>3.1825637997711209E-2</v>
       </c>
       <c r="N7" s="244" t="str">
         <v>#N/A</v>
@@ -21801,7 +21750,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="244">
-        <v>3.2329549552616528E-2</v>
+        <v>3.1825637997711209E-2</v>
       </c>
       <c r="Q7" s="244">
         <v>0</v>
@@ -21840,25 +21789,25 @@
     </row>
     <row r="8" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="237">
-        <v>0.92143275179637318</v>
+        <v>0.92319139827288144</v>
       </c>
       <c r="B8" s="238">
         <v>42955</v>
       </c>
       <c r="C8" s="239">
-        <v>17150.044374726116</v>
+        <v>16714.38923442148</v>
       </c>
       <c r="D8" s="239">
         <v>1000000</v>
       </c>
       <c r="E8" s="238">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="F8" s="238">
         <v>42955</v>
       </c>
       <c r="G8" s="240">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H8" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21867,16 +21816,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="238">
-        <v>42772</v>
+        <v>42774</v>
       </c>
       <c r="K8" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L8" s="243">
-        <v>0.50136986301369868</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M8" s="244">
-        <v>3.4206372659972846E-2</v>
+        <v>3.37058125445516E-2</v>
       </c>
       <c r="N8" s="244" t="str">
         <v>#N/A</v>
@@ -21885,7 +21834,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="244">
-        <v>3.4206372659972846E-2</v>
+        <v>3.37058125445516E-2</v>
       </c>
       <c r="Q8" s="244">
         <v>0</v>
@@ -21924,13 +21873,13 @@
     </row>
     <row r="9" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="237">
-        <v>0.90679493634089159</v>
+        <v>0.90848563416936845</v>
       </c>
       <c r="B9" s="238">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="C9" s="239">
-        <v>18030.368482273796</v>
+        <v>18028.221537314203</v>
       </c>
       <c r="D9" s="239">
         <v>1000000</v>
@@ -21939,10 +21888,10 @@
         <v>42955</v>
       </c>
       <c r="F9" s="238">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="G9" s="240">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H9" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21957,10 +21906,10 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L9" s="243">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M9" s="244">
-        <v>3.6159804923241404E-2</v>
+        <v>3.576250467999828E-2</v>
       </c>
       <c r="N9" s="244" t="str">
         <v>#N/A</v>
@@ -21969,7 +21918,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="244">
-        <v>3.6159804923241404E-2</v>
+        <v>3.576250467999828E-2</v>
       </c>
       <c r="Q9" s="244">
         <v>0</v>
@@ -22008,25 +21957,25 @@
     </row>
     <row r="10" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="237">
-        <v>0.89180866948193593</v>
+        <v>0.89360865189861183</v>
       </c>
       <c r="B10" s="238">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="C10" s="239">
-        <v>18792.361275124622</v>
+        <v>18557.049765872915</v>
       </c>
       <c r="D10" s="239">
         <v>1000000</v>
       </c>
       <c r="E10" s="238">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="F10" s="238">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="G10" s="240">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H10" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22035,16 +21984,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="238">
-        <v>43137</v>
+        <v>43139</v>
       </c>
       <c r="K10" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L10" s="243">
-        <v>0.49863013698630138</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M10" s="244">
-        <v>3.768797728253015E-2</v>
+        <v>3.7421674942229907E-2</v>
       </c>
       <c r="N10" s="244" t="str">
         <v>#N/A</v>
@@ -22053,10 +22002,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="244">
-        <v>3.7687977282530156E-2</v>
+        <v>3.7421674942229907E-2</v>
       </c>
       <c r="Q10" s="244">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R10" s="244">
         <v>0</v>
@@ -22092,25 +22041,25 @@
     </row>
     <row r="11" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="237">
-        <v>0.87635138893012232</v>
+        <v>0.87810972118544339</v>
       </c>
       <c r="B11" s="238">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="C11" s="239">
-        <v>19468.516985524657</v>
+        <v>19507.295201224297</v>
       </c>
       <c r="D11" s="239">
         <v>1000000</v>
       </c>
       <c r="E11" s="238">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="F11" s="238">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="G11" s="240">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H11" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22119,16 +22068,16 @@
         <v>0</v>
       </c>
       <c r="J11" s="238">
-        <v>43319</v>
+        <v>43320</v>
       </c>
       <c r="K11" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L11" s="243">
-        <v>0.50136986301369868</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M11" s="244">
-        <v>3.8830648632330593E-2</v>
+        <v>3.8696536676341667E-2</v>
       </c>
       <c r="N11" s="244" t="str">
         <v>#N/A</v>
@@ -22137,10 +22086,10 @@
         <v>1</v>
       </c>
       <c r="P11" s="244">
-        <v>3.8830648632330586E-2</v>
+        <v>3.8696536676341667E-2</v>
       </c>
       <c r="Q11" s="244">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R11" s="244">
         <v>0</v>
@@ -22176,22 +22125,22 @@
     </row>
     <row r="12" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="237">
-        <v>0.86080364957416167</v>
+        <v>0.86258376609713372</v>
       </c>
       <c r="B12" s="238">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="C12" s="239">
-        <v>19934.743335291438</v>
+        <v>19876.685812506563</v>
       </c>
       <c r="D12" s="239">
         <v>1000000</v>
       </c>
       <c r="E12" s="238">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="F12" s="238">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="G12" s="240">
         <v>181</v>
@@ -22203,7 +22152,7 @@
         <v>0</v>
       </c>
       <c r="J12" s="238">
-        <v>43502</v>
+        <v>43504</v>
       </c>
       <c r="K12" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
@@ -22212,7 +22161,7 @@
         <v>0.49589041095890413</v>
       </c>
       <c r="M12" s="244">
-        <v>4.0199896781112569E-2</v>
+        <v>4.0082819456159643E-2</v>
       </c>
       <c r="N12" s="244" t="str">
         <v>#N/A</v>
@@ -22221,10 +22170,10 @@
         <v>1</v>
       </c>
       <c r="P12" s="244">
-        <v>4.0199896781112569E-2</v>
+        <v>4.008281945615965E-2</v>
       </c>
       <c r="Q12" s="244">
-        <v>0</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="R12" s="244">
         <v>0</v>
@@ -22260,25 +22209,25 @@
     </row>
     <row r="13" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="237">
-        <v>0.84481831838569088</v>
+        <v>0.84638478006872575</v>
       </c>
       <c r="B13" s="238">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="C13" s="239">
-        <v>21084.250092414884</v>
+        <v>21223.909808522065</v>
       </c>
       <c r="D13" s="239">
         <v>1000000</v>
       </c>
       <c r="E13" s="238">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="F13" s="238">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="G13" s="240">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H13" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22287,16 +22236,16 @@
         <v>0</v>
       </c>
       <c r="J13" s="238">
-        <v>43683</v>
+        <v>43685</v>
       </c>
       <c r="K13" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L13" s="243">
-        <v>0.50410958904109593</v>
+        <v>0.50958904109589043</v>
       </c>
       <c r="M13" s="244">
-        <v>4.1824735237670822E-2</v>
+        <v>4.1649070323175018E-2</v>
       </c>
       <c r="N13" s="244" t="str">
         <v>#N/A</v>
@@ -22305,10 +22254,10 @@
         <v>1</v>
       </c>
       <c r="P13" s="244">
-        <v>4.1824735237670815E-2</v>
+        <v>4.1649070323175025E-2</v>
       </c>
       <c r="Q13" s="244">
-        <v>6.9388939039072284E-18</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="R13" s="244">
         <v>0</v>
@@ -22344,22 +22293,22 @@
     </row>
     <row r="14" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="237">
-        <v>0.82862259521329318</v>
+        <v>0.83012725902555851</v>
       </c>
       <c r="B14" s="238">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="C14" s="239">
-        <v>21477.27167384006</v>
+        <v>21421.123322118652</v>
       </c>
       <c r="D14" s="239">
         <v>1000000</v>
       </c>
       <c r="E14" s="238">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="F14" s="238">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="G14" s="240">
         <v>182</v>
@@ -22371,7 +22320,7 @@
         <v>0</v>
       </c>
       <c r="J14" s="238">
-        <v>43867</v>
+        <v>43871</v>
       </c>
       <c r="K14" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
@@ -22380,7 +22329,7 @@
         <v>0.49863013698630138</v>
       </c>
       <c r="M14" s="244">
-        <v>4.3072550334899019E-2</v>
+        <v>4.2959945124029161E-2</v>
       </c>
       <c r="N14" s="244" t="str">
         <v>#N/A</v>
@@ -22389,7 +22338,7 @@
         <v>1</v>
       </c>
       <c r="P14" s="244">
-        <v>4.3072550334899019E-2</v>
+        <v>4.2959945124029161E-2</v>
       </c>
       <c r="Q14" s="244">
         <v>0</v>
@@ -22428,25 +22377,25 @@
     </row>
     <row r="15" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="237">
-        <v>0.81160713553623487</v>
+        <v>0.8134325054127004</v>
       </c>
       <c r="B15" s="238">
         <v>44235</v>
       </c>
       <c r="C15" s="239">
-        <v>22365.563549803457</v>
+        <v>21929.369050826204</v>
       </c>
       <c r="D15" s="239">
         <v>1000000</v>
       </c>
       <c r="E15" s="238">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="F15" s="238">
         <v>44235</v>
       </c>
       <c r="G15" s="240">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H15" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22455,16 +22404,16 @@
         <v>0</v>
       </c>
       <c r="J15" s="238">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="K15" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L15" s="243">
-        <v>0.50958904109589043</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M15" s="244">
-        <v>4.3889412342356243E-2</v>
+        <v>4.3979229140393213E-2</v>
       </c>
       <c r="N15" s="244" t="str">
         <v>#N/A</v>
@@ -22473,10 +22422,10 @@
         <v>1</v>
       </c>
       <c r="P15" s="244">
-        <v>4.3889412342356243E-2</v>
+        <v>4.397922914039322E-2</v>
       </c>
       <c r="Q15" s="244">
-        <v>0</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="R15" s="244">
         <v>0</v>
@@ -22512,13 +22461,13 @@
     </row>
     <row r="16" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="237">
-        <v>0.79544497159972916</v>
+        <v>0.79692238577986874</v>
       </c>
       <c r="B16" s="238">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="C16" s="239">
-        <v>21830.499433272089</v>
+        <v>22386.046814613092</v>
       </c>
       <c r="D16" s="239">
         <v>1000000</v>
@@ -22527,10 +22476,10 @@
         <v>44235</v>
       </c>
       <c r="F16" s="238">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="G16" s="240">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H16" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22545,10 +22494,10 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L16" s="243">
-        <v>0.49041095890410957</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M16" s="244">
-        <v>4.4514705548292247E-2</v>
+        <v>4.4895093886449335E-2</v>
       </c>
       <c r="N16" s="244" t="str">
         <v>#N/A</v>
@@ -22557,7 +22506,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="244">
-        <v>4.4514705548292247E-2</v>
+        <v>4.4895093886449335E-2</v>
       </c>
       <c r="Q16" s="244">
         <v>0</v>
@@ -22596,25 +22545,25 @@
     </row>
     <row r="17" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="237">
-        <v>0.77951065610534276</v>
+        <v>0.78102890658709501</v>
       </c>
       <c r="B17" s="238">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="C17" s="239">
-        <v>22869.972017331984</v>
+        <v>22910.739816467409</v>
       </c>
       <c r="D17" s="239">
         <v>1000000</v>
       </c>
       <c r="E17" s="238">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="F17" s="238">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="G17" s="240">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H17" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22623,16 +22572,16 @@
         <v>0</v>
       </c>
       <c r="J17" s="238">
-        <v>44414</v>
+        <v>44417</v>
       </c>
       <c r="K17" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L17" s="243">
-        <v>0.50684931506849318</v>
+        <v>0.50136986301369868</v>
       </c>
       <c r="M17" s="244">
-        <v>4.5121836682844182E-2</v>
+        <v>4.569628433339127E-2</v>
       </c>
       <c r="N17" s="244" t="str">
         <v>#N/A</v>
@@ -22641,7 +22590,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="244">
-        <v>4.5121836682844182E-2</v>
+        <v>4.569628433339127E-2</v>
       </c>
       <c r="Q17" s="244">
         <v>0</v>
@@ -22680,25 +22629,25 @@
     </row>
     <row r="18" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="237">
-        <v>0.76413364028636954</v>
+        <v>0.76564045846940665</v>
       </c>
       <c r="B18" s="238">
         <v>44781</v>
       </c>
       <c r="C18" s="239">
-        <v>22831.17987391381</v>
+        <v>22872.337787458451</v>
       </c>
       <c r="D18" s="239">
         <v>1000000</v>
       </c>
       <c r="E18" s="238">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="F18" s="238">
         <v>44781</v>
       </c>
       <c r="G18" s="240">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H18" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22707,16 +22656,16 @@
         <v>0</v>
       </c>
       <c r="J18" s="238">
-        <v>44599</v>
+        <v>44600</v>
       </c>
       <c r="K18" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L18" s="243">
-        <v>0.49863013698630138</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M18" s="244">
-        <v>4.5787805791090881E-2</v>
+        <v>4.6123775096255995E-2</v>
       </c>
       <c r="N18" s="244" t="str">
         <v>#N/A</v>
@@ -22725,7 +22674,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="244">
-        <v>4.5787805791090881E-2</v>
+        <v>4.6123775096255995E-2</v>
       </c>
       <c r="Q18" s="244">
         <v>0</v>
@@ -22764,13 +22713,13 @@
     </row>
     <row r="19" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="237">
-        <v>0.74852864113593476</v>
+        <v>0.74986498717119976</v>
       </c>
       <c r="B19" s="238">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="C19" s="239">
-        <v>23187.218703049068</v>
+        <v>23335.465339302085</v>
       </c>
       <c r="D19" s="239">
         <v>1000000</v>
@@ -22779,10 +22728,10 @@
         <v>44781</v>
       </c>
       <c r="F19" s="238">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="G19" s="240">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H19" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22797,10 +22746,10 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L19" s="243">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M19" s="244">
-        <v>4.6501839706664341E-2</v>
+        <v>4.6290461135028591E-2</v>
       </c>
       <c r="N19" s="244" t="str">
         <v>#N/A</v>
@@ -22809,10 +22758,10 @@
         <v>1</v>
       </c>
       <c r="P19" s="244">
-        <v>4.6501839706664348E-2</v>
+        <v>4.6290461135028591E-2</v>
       </c>
       <c r="Q19" s="244">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R19" s="244">
         <v>0</v>
@@ -22848,25 +22797,25 @@
     </row>
     <row r="20" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="237">
-        <v>0.7326415617948786</v>
+        <v>0.73411965313311145</v>
       </c>
       <c r="B20" s="238">
         <v>45146</v>
       </c>
       <c r="C20" s="239">
-        <v>23567.420210947046</v>
+        <v>23184.476417786875</v>
       </c>
       <c r="D20" s="239">
         <v>1000000</v>
       </c>
       <c r="E20" s="238">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="F20" s="238">
         <v>45146</v>
       </c>
       <c r="G20" s="240">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H20" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22875,16 +22824,16 @@
         <v>0</v>
       </c>
       <c r="J20" s="238">
-        <v>44963</v>
+        <v>44965</v>
       </c>
       <c r="K20" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L20" s="243">
-        <v>0.50136986301369868</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M20" s="244">
-        <v>4.7006056704894376E-2</v>
+        <v>4.6753225925371317E-2</v>
       </c>
       <c r="N20" s="244" t="str">
         <v>#N/A</v>
@@ -22893,7 +22842,7 @@
         <v>1</v>
       </c>
       <c r="P20" s="244">
-        <v>4.7006056704894369E-2</v>
+        <v>4.675322592537131E-2</v>
       </c>
       <c r="Q20" s="244">
         <v>6.9388939039072284E-18</v>
@@ -22932,13 +22881,13 @@
     </row>
     <row r="21" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="237">
-        <v>0.71681099301552698</v>
+        <v>0.71794182972811249</v>
       </c>
       <c r="B21" s="238">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="C21" s="239">
-        <v>23601.260658036914</v>
+        <v>23987.610087518704</v>
       </c>
       <c r="D21" s="239">
         <v>1000000</v>
@@ -22947,10 +22896,10 @@
         <v>45146</v>
       </c>
       <c r="F21" s="238">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="G21" s="240">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H21" s="241" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22965,10 +22914,10 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L21" s="243">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M21" s="244">
-        <v>4.7332198572436666E-2</v>
+        <v>4.758411783665395E-2</v>
       </c>
       <c r="N21" s="244" t="str">
         <v>#N/A</v>
@@ -22977,7 +22926,7 @@
         <v>1</v>
       </c>
       <c r="P21" s="244">
-        <v>4.7332198572436673E-2</v>
+        <v>4.7584117836653957E-2</v>
       </c>
       <c r="Q21" s="244">
         <v>-6.9388939039072284E-18</v>
@@ -23016,22 +22965,22 @@
     </row>
     <row r="22" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="237">
-        <v>0.70112984314388349</v>
+        <v>0.70208555969117814</v>
       </c>
       <c r="B22" s="238">
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="C22" s="239">
-        <v>23894.381712262992</v>
+        <v>24089.917919180025</v>
       </c>
       <c r="D22" s="239">
         <v>1000000</v>
       </c>
       <c r="E22" s="238">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="F22" s="238">
-        <v>45510</v>
+        <v>45512</v>
       </c>
       <c r="G22" s="240">
         <v>182</v>
@@ -23043,7 +22992,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="238">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="K22" s="240" t="str">
         <v>Actual/365 (Fixed)</v>
@@ -23052,7 +23001,7 @@
         <v>0.49863013698630138</v>
       </c>
       <c r="M22" s="244">
-        <v>4.7920051236131821E-2</v>
+        <v>4.8312198024729171E-2</v>
       </c>
       <c r="N22" s="244" t="str">
         <v>#N/A</v>
@@ -23061,7 +23010,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="244">
-        <v>4.7920051236131821E-2</v>
+        <v>4.8312198024729171E-2</v>
       </c>
       <c r="Q22" s="244">
         <v>0</v>

</xml_diff>

<commit_message>
AUD 1M Curve + Contribution for UAT
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/AUDSwap.xlsx
+++ b/QuantLibXL/Data2/XLS/AUDSwap.xlsx
@@ -1641,6 +1641,7 @@
     <xf numFmtId="168" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1657,7 +1658,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1765,14 +1765,14 @@
       <sheetData sheetId="7">
         <row r="7">
           <cell r="D7" t="str">
-            <v>Z4</v>
+            <v>F5</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="8">
         <row r="7">
           <cell r="D7" t="str">
-            <v>V4</v>
+            <v>X4</v>
           </cell>
         </row>
       </sheetData>
@@ -2126,7 +2126,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="216">
-        <v>41858.779293981483</v>
+        <v>41883.627685185187</v>
       </c>
       <c r="E3" s="212"/>
     </row>
@@ -2182,7 +2182,7 @@
       </c>
       <c r="D10" s="266">
         <f>IF(D9,_xll.qlSettingsEvaluationDate(Trigger),_xll.qlCalendarAdvance(Calendar,_xll.qlSettingsEvaluationDate(Trigger),"1d","f",,Trigger))</f>
-        <v>41858</v>
+        <v>41883</v>
       </c>
       <c r="E10" s="212"/>
     </row>
@@ -2210,7 +2210,7 @@
   <dimension ref="A1:T87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -2281,20 +2281,20 @@
       <c r="A2" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="267" t="s">
+      <c r="B2" s="268" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="268"/>
+      <c r="C2" s="269"/>
       <c r="D2" s="59" t="s">
         <v>46</v>
       </c>
       <c r="E2" s="60" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="267" t="s">
+      <c r="F2" s="268" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="268"/>
+      <c r="G2" s="269"/>
       <c r="H2" s="57" t="s">
         <v>46</v>
       </c>
@@ -2307,10 +2307,10 @@
       <c r="K2" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="267" t="s">
+      <c r="L2" s="268" t="s">
         <v>52</v>
       </c>
-      <c r="M2" s="268"/>
+      <c r="M2" s="269"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="J3" s="102" t="str">
         <f>FirstLegCF</f>
-        <v>obj_00945#0055</v>
+        <v>obj_003fc#0001</v>
       </c>
       <c r="K3" s="29" t="b">
         <f>C27</f>
@@ -2359,14 +2359,14 @@
       </c>
       <c r="L3" s="139">
         <f>EvaluationDate</f>
-        <v>41858</v>
+        <v>41883</v>
       </c>
       <c r="M3" s="140">
         <v>0</v>
       </c>
       <c r="N3" s="1" t="str">
         <f>_xll.qlLeg(,M3,L3,,,EvaluationDate)</f>
-        <v>obj_0093b#0000</v>
+        <v>obj_003f3#0000</v>
       </c>
       <c r="O3" s="1" t="b">
         <v>1</v>
@@ -2384,32 +2384,32 @@
       <c r="B4" s="265"/>
       <c r="C4" s="98">
         <f>IF(ISBLANK(B4),D4,B4)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="D4" s="133">
         <f t="shared" si="1"/>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="E4" s="134">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlInterestRateIndexValueDate(C24,EvaluationDate),"1D","f",,Trigger)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="F4" s="144"/>
       <c r="G4" s="65">
         <f>IF(ISBLANK(F4),H4,F4)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="H4" s="133">
         <f>IF(ISBLANK(B4),I4,C4)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="I4" s="134">
         <f>_xll.qlCalendarAdvance(Calendar,_xll.qlInterestRateIndexValueDate(G24,EvaluationDate),"1D","f",,Trigger)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="J4" s="21" t="str">
         <f>SecondLegCF</f>
-        <v>obj_00943#0044</v>
+        <v>obj_003fd#0001</v>
       </c>
       <c r="K4" s="27" t="b">
         <f>G27</f>
@@ -2417,14 +2417,14 @@
       </c>
       <c r="L4" s="141">
         <f>_xll.qlCalendarAdvance($C$3,L3,"1D","f")</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="M4" s="142">
         <v>0</v>
       </c>
       <c r="N4" s="1" t="str">
         <f>_xll.qlLeg(,M4,L4,,,EvaluationDate)</f>
-        <v>obj_0093e#0002</v>
+        <v>obj_003f6#0001</v>
       </c>
       <c r="O4" s="1" t="b">
         <f t="shared" ref="O4:O26" si="2">NOT(M4=0)</f>
@@ -2459,7 +2459,7 @@
         <v>#N/A</v>
       </c>
       <c r="H5" s="133" t="e">
-        <f t="shared" ref="H4:H13" si="4">IF(ISBLANK(B5),I5,C5)</f>
+        <f t="shared" ref="H5:H13" si="4">IF(ISBLANK(B5),I5,C5)</f>
         <v>#N/A</v>
       </c>
       <c r="I5" s="134" t="e">
@@ -2468,21 +2468,21 @@
       </c>
       <c r="J5" s="30" t="str">
         <f>AdditionalCF</f>
-        <v>obj_00944#0005</v>
+        <v>obj_003f9#0001</v>
       </c>
       <c r="K5" s="30" t="b">
         <v>0</v>
       </c>
       <c r="L5" s="141">
         <f>_xll.qlCalendarAdvance($C$3,L4,"1D","f")</f>
-        <v>41862</v>
+        <v>41885</v>
       </c>
       <c r="M5" s="142">
         <v>0</v>
       </c>
       <c r="N5" s="1" t="str">
         <f>_xll.qlLeg(,M5,L5,,,EvaluationDate)</f>
-        <v>obj_0093d#0002</v>
+        <v>obj_003f5#0001</v>
       </c>
       <c r="O5" s="1" t="b">
         <f t="shared" si="2"/>
@@ -2528,14 +2528,14 @@
       <c r="K6" s="5"/>
       <c r="L6" s="141">
         <f>_xll.qlCalendarAdvance($C$3,L5,"1D","f")</f>
-        <v>41863</v>
+        <v>41886</v>
       </c>
       <c r="M6" s="142">
         <v>0</v>
       </c>
       <c r="N6" s="1" t="str">
         <f>_xll.qlLeg(,M6,L6,,,EvaluationDate)</f>
-        <v>obj_0093f#0002</v>
+        <v>obj_003f7#0001</v>
       </c>
       <c r="O6" s="1" t="b">
         <f t="shared" si="2"/>
@@ -2602,28 +2602,28 @@
       <c r="B8" s="4"/>
       <c r="C8" s="98">
         <f t="shared" si="0"/>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="D8" s="133">
         <f t="shared" si="1"/>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="E8" s="134">
         <f>_xll.qlCalendarAdvance("NULLCALENDAR",C$4,C$7,"Unadjusted")</f>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="F8" s="144"/>
       <c r="G8" s="65">
         <f t="shared" si="3"/>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="H8" s="133">
         <f t="shared" si="4"/>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="I8" s="134">
         <f>_xll.qlCalendarAdvance("NULLCALENDAR",G$4,G$7,"Unadjusted")</f>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
@@ -2898,21 +2898,21 @@
       <c r="B14" s="17"/>
       <c r="C14" s="101" t="str">
         <f t="shared" si="0"/>
-        <v>obj_00941#0013</v>
+        <v>obj_003fb#0001</v>
       </c>
       <c r="D14" s="137" t="str">
         <f>_xll.qlSchedule(,C4,C8,C9,C3,C10,C11,C12,C13,C5,C6)</f>
-        <v>obj_00941#0013</v>
+        <v>obj_003fb#0001</v>
       </c>
       <c r="E14" s="138"/>
       <c r="F14" s="114"/>
       <c r="G14" s="69" t="str">
         <f>IF(ISBLANK(F14),H14,F14)</f>
-        <v>obj_00940#0005</v>
+        <v>obj_003fa#0001</v>
       </c>
       <c r="H14" s="137" t="str">
         <f>_xll.qlSchedule(,G4,G8,G9,G3,G10,G11,G12,G13,G5,G6)</f>
-        <v>obj_00940#0005</v>
+        <v>obj_003fa#0001</v>
       </c>
       <c r="I14" s="138"/>
       <c r="J14" s="5"/>
@@ -3535,14 +3535,14 @@
       <c r="K27" s="5"/>
       <c r="L27" s="141">
         <f>_xll.qlCalendarAdjust($C$3,E8,$C$11)</f>
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="M27" s="142">
         <v>0</v>
       </c>
       <c r="N27" s="1" t="str">
         <f>_xll.qlLeg(,M27,L27,,,EvaluationDate)</f>
-        <v>obj_00942#0005</v>
+        <v>obj_003f8#0001</v>
       </c>
       <c r="O27" s="1" t="b">
         <v>1</v>
@@ -3560,21 +3560,21 @@
       <c r="B28" s="104"/>
       <c r="C28" s="105" t="str">
         <f>IF(ISBLANK(B28),D28,B28)</f>
-        <v>obj_00945#0055</v>
+        <v>obj_003fc#0001</v>
       </c>
       <c r="D28" s="129" t="str">
         <f>_xll.qlIborLeg(B28,C16,_xll.ohPack(FirstLegAdmortization!Effective),C14,C19,C20,C21,C22,C23,C24,C25,C26)</f>
-        <v>obj_00945#0055</v>
+        <v>obj_003fc#0001</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="114"/>
       <c r="G28" s="74" t="str">
         <f t="shared" si="6"/>
-        <v>obj_00943#0044</v>
+        <v>obj_003fd#0001</v>
       </c>
       <c r="H28" s="129" t="str">
         <f>_xll.qlIborLeg(F28,G16,_xll.ohPack(SecondLegAdmortization!Effective),G14,G19,G20,G21,G22,G23,G24,G25,G26)</f>
-        <v>obj_00943#0044</v>
+        <v>obj_003fd#0001</v>
       </c>
       <c r="I28" s="15"/>
       <c r="J28" s="5"/>
@@ -3582,11 +3582,11 @@
       <c r="L28" s="143"/>
       <c r="M28" s="64" t="str">
         <f>IF(ISBLANK(L28),N28,L28)</f>
-        <v>obj_00944#0005</v>
+        <v>obj_003f9#0001</v>
       </c>
       <c r="N28" s="26" t="str">
         <f>_xll.qlMultiPhaseLeg(,_xll.ohFilter(N3:N27,O3:O27),FALSE)</f>
-        <v>obj_00944#0005</v>
+        <v>obj_003f9#0001</v>
       </c>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3602,7 +3602,7 @@
       <c r="B29" s="131"/>
       <c r="C29" s="19" t="str">
         <f>_xll.qlSwap(B29,$J$3:$J$5,$K$3:$K$5)</f>
-        <v>obj_00946#0050</v>
+        <v>obj_003fe#0001</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="9"/>
@@ -3937,11 +3937,11 @@
       <c r="B40" s="28"/>
       <c r="C40" s="166">
         <f>IF(ISBLANK(B40),D40,B40)</f>
-        <v>41858</v>
+        <v>41883</v>
       </c>
       <c r="D40" s="147">
         <f>EvaluationDate</f>
-        <v>41858</v>
+        <v>41883</v>
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="11"/>
@@ -3967,11 +3967,11 @@
       <c r="B41" s="28"/>
       <c r="C41" s="166">
         <f>IF(ISBLANK(B41),D41,B41)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="D41" s="147">
         <f>E4</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
@@ -3997,11 +3997,11 @@
       <c r="B42" s="150"/>
       <c r="C42" s="73" t="str">
         <f>IF(ISBLANK(B42),D42,B42)</f>
-        <v>obj_0093c#0002</v>
+        <v>obj_003f4#0001</v>
       </c>
       <c r="D42" s="148" t="str">
         <f>_xll.qlDiscountingSwapEngine(,DiscountCurve,IncludeSettlementDate,SettlementDate,NPVDate)</f>
-        <v>obj_0093c#0002</v>
+        <v>obj_003f4#0001</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -4076,7 +4076,7 @@
       <c r="B45" s="82"/>
       <c r="C45" s="83">
         <f>_xll.ohTrigger(AllTriggers,C43,ISERROR(C35),ISERROR(G35))</f>
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="D45" s="20"/>
       <c r="E45" s="20"/>
@@ -4125,7 +4125,7 @@
       <c r="B47" s="84"/>
       <c r="C47" s="85">
         <f>_xll.qlInstrumentNPV(SwapID,C45)</f>
-        <v>326659.31446107215</v>
+        <v>316338.00719063281</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="9"/>
@@ -4174,14 +4174,14 @@
       <c r="B49" s="151"/>
       <c r="C49" s="152">
         <f>C$25-NPV/C$51/10000</f>
-        <v>3.8350000000040844E-2</v>
+        <v>3.6974999999997024E-2</v>
       </c>
       <c r="D49" s="155"/>
       <c r="E49" s="155"/>
       <c r="F49" s="151"/>
       <c r="G49" s="152">
         <f>G$25-NPV/G$51/10000</f>
-        <v>-3.8350000000040844E-2</v>
+        <v>-3.6974999999997024E-2</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -4211,7 +4211,7 @@
       <c r="F50" s="91"/>
       <c r="G50" s="156">
         <f>_xll.qlSwapLegNPV(SwapID,1,$C$45)</f>
-        <v>326659.31446107215</v>
+        <v>316338.00719063281</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
@@ -4237,14 +4237,14 @@
       <c r="B51" s="151"/>
       <c r="C51" s="158">
         <f>_xll.qlSwapLegBPS(SwapID,0,C45)</f>
-        <v>-851.78439233565655</v>
+        <v>-855.54565839258487</v>
       </c>
       <c r="D51" s="155"/>
       <c r="E51" s="155"/>
       <c r="F51" s="151"/>
       <c r="G51" s="158">
         <f>_xll.qlSwapLegBPS(SwapID,1,C45)</f>
-        <v>851.78439233565655</v>
+        <v>855.54565839258487</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
@@ -5025,11 +5025,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1 F1 I1">
       <formula1>"EUR,USD,GBP,JPY,CHF,AUD,CNY,CNH,HKD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24 F24">
-      <formula1>"AudBBSW3M,AudBBSW6M,Euribor3M,Euribor6M"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37">
       <formula1>"AUDON,AUDSTD,AUDEURBASOIS,AUDEURBASSTD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F24 B24">
+      <formula1>"AudBBSW1M,AudBBSW3M,AudBBSW6M,Euribor3M,Euribor6M"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5064,7 +5064,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="35" t="str">
         <f>Pricing!$C$14</f>
-        <v>obj_00941#0013</v>
+        <v>obj_003fb#0001</v>
       </c>
       <c r="C1" s="34" t="str">
         <f>UPPER(Pricing!$C$18)</f>
@@ -5121,7 +5121,7 @@
       </c>
       <c r="B4" s="41">
         <f t="array" ref="B4:B123">_xll.qlScheduleDates(Schedule)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="C4" s="43">
         <f t="array" ref="C4:C123">IF(Type="MIRROR",E4:E123,IF(Type="CUSTOM",F4:F123,IF(Type="STEP",G4:G123,IF(Type="FRENCH",H4:H123,D4:D123))))</f>
@@ -5157,7 +5157,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="41">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="C5" s="43">
         <v>1000000</v>
@@ -5191,7 +5191,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="41">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="C6" s="43">
         <v>1000000</v>
@@ -5225,7 +5225,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="41">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="C7" s="43">
         <v>1000000</v>
@@ -5259,7 +5259,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="41">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="C8" s="43">
         <v>1000000</v>
@@ -5293,7 +5293,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="41">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="C9" s="43">
         <v>1000000</v>
@@ -5327,7 +5327,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="41">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="C10" s="43">
         <v>1000000</v>
@@ -5361,7 +5361,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="41">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="C11" s="43">
         <v>1000000</v>
@@ -5395,7 +5395,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="41">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="C12" s="43">
         <v>1000000</v>
@@ -5429,7 +5429,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="41">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="C13" s="43">
         <v>1000000</v>
@@ -5463,7 +5463,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="41">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="C14" s="43">
         <v>1000000</v>
@@ -5497,7 +5497,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="41">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="C15" s="43">
         <v>1000000</v>
@@ -5531,7 +5531,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="41">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="C16" s="43">
         <v>1000000</v>
@@ -5565,7 +5565,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="41">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="C17" s="43">
         <v>1000000</v>
@@ -5599,7 +5599,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="41">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="C18" s="43">
         <v>1000000</v>
@@ -5633,7 +5633,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="41">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="C19" s="43">
         <v>1000000</v>
@@ -5667,7 +5667,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="41">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="C20" s="43">
         <v>1000000</v>
@@ -5701,7 +5701,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="41">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="C21" s="43">
         <v>1000000</v>
@@ -5735,7 +5735,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="41">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="C22" s="43">
         <v>1000000</v>
@@ -5769,7 +5769,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="41">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="C23" s="43">
         <v>1000000</v>
@@ -5803,7 +5803,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="41">
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="C24" s="43" t="e">
         <v>#N/A</v>
@@ -9234,29 +9234,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="270" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="270"/>
-      <c r="C1" s="270"/>
-      <c r="D1" s="270"/>
-      <c r="E1" s="270"/>
-      <c r="F1" s="270"/>
-      <c r="G1" s="270"/>
-      <c r="H1" s="270"/>
-      <c r="I1" s="270"/>
-      <c r="J1" s="270"/>
-      <c r="K1" s="270"/>
-      <c r="L1" s="270"/>
-      <c r="M1" s="270"/>
-      <c r="N1" s="270"/>
-      <c r="O1" s="270"/>
-      <c r="P1" s="270"/>
-      <c r="Q1" s="270"/>
-      <c r="R1" s="270"/>
-      <c r="S1" s="270"/>
-      <c r="T1" s="270"/>
-      <c r="U1" s="271"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="271"/>
+      <c r="F1" s="271"/>
+      <c r="G1" s="271"/>
+      <c r="H1" s="271"/>
+      <c r="I1" s="271"/>
+      <c r="J1" s="271"/>
+      <c r="K1" s="271"/>
+      <c r="L1" s="271"/>
+      <c r="M1" s="271"/>
+      <c r="N1" s="271"/>
+      <c r="O1" s="271"/>
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="272"/>
     </row>
     <row r="2" spans="1:23" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="182" t="s">
@@ -9327,10 +9327,10 @@
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="185">
         <f t="array" ref="A3:A122">_xll.qlYieldTSDiscount(DiscountCurve,_xll.ohPack(B3:B122))</f>
-        <v>0.98762977471753821</v>
+        <v>0.98781996868675226</v>
       </c>
       <c r="B3" s="186">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="C3" s="187">
         <v>0</v>
@@ -9339,13 +9339,13 @@
         <v>1000000</v>
       </c>
       <c r="E3" s="186">
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="F3" s="186">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="G3" s="188">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H3" s="189" t="str">
         <v>#N/A</v>
@@ -9360,7 +9360,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L3" s="191">
-        <v>0.50684931506849318</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M3" s="192">
         <v>0</v>
@@ -9389,15 +9389,15 @@
       <c r="U3" s="194" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V3" s="275"/>
-      <c r="W3" s="275"/>
+      <c r="V3" s="267"/>
+      <c r="W3" s="267"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" s="195">
-        <v>0.97593905629035904</v>
+        <v>0.97589522175637922</v>
       </c>
       <c r="B4" s="174">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="C4" s="176">
         <v>0</v>
@@ -9406,13 +9406,13 @@
         <v>1000000</v>
       </c>
       <c r="E4" s="174">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="F4" s="174">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="G4" s="175">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H4" s="177" t="str">
         <v>#N/A</v>
@@ -9427,7 +9427,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L4" s="179">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M4" s="180">
         <v>0</v>
@@ -9456,15 +9456,15 @@
       <c r="U4" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V4" s="275"/>
-      <c r="W4" s="275"/>
+      <c r="V4" s="267"/>
+      <c r="W4" s="267"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="195">
-        <v>0.963823130511412</v>
+        <v>0.96381080870229641</v>
       </c>
       <c r="B5" s="174">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="C5" s="176">
         <v>0</v>
@@ -9473,10 +9473,10 @@
         <v>1000000</v>
       </c>
       <c r="E5" s="174">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="F5" s="174">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="G5" s="175">
         <v>182</v>
@@ -9523,15 +9523,15 @@
       <c r="U5" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V5" s="275"/>
-      <c r="W5" s="275"/>
+      <c r="V5" s="267"/>
+      <c r="W5" s="267"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" s="195">
-        <v>0.95091964847149946</v>
+        <v>0.95092413549530208</v>
       </c>
       <c r="B6" s="174">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="C6" s="176">
         <v>0</v>
@@ -9540,13 +9540,13 @@
         <v>1000000</v>
       </c>
       <c r="E6" s="174">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="F6" s="174">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="G6" s="175">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H6" s="177" t="str">
         <v>#N/A</v>
@@ -9561,7 +9561,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L6" s="179">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M6" s="180">
         <v>0</v>
@@ -9590,15 +9590,15 @@
       <c r="U6" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V6" s="275"/>
-      <c r="W6" s="275"/>
+      <c r="V6" s="267"/>
+      <c r="W6" s="267"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" s="195">
-        <v>0.9372080274699961</v>
+        <v>0.93760752950670501</v>
       </c>
       <c r="B7" s="174">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="C7" s="176">
         <v>0</v>
@@ -9607,13 +9607,13 @@
         <v>1000000</v>
       </c>
       <c r="E7" s="174">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="F7" s="174">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="G7" s="175">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H7" s="177" t="str">
         <v>#N/A</v>
@@ -9628,7 +9628,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L7" s="179">
-        <v>0.50410958904109593</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M7" s="180">
         <v>0</v>
@@ -9657,15 +9657,15 @@
       <c r="U7" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V7" s="275"/>
-      <c r="W7" s="275"/>
+      <c r="V7" s="267"/>
+      <c r="W7" s="267"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" s="195">
-        <v>0.92319139827288144</v>
+        <v>0.92348093763004924</v>
       </c>
       <c r="B8" s="174">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="C8" s="176">
         <v>0</v>
@@ -9674,13 +9674,13 @@
         <v>1000000</v>
       </c>
       <c r="E8" s="174">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="F8" s="174">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="G8" s="175">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H8" s="177" t="str">
         <v>#N/A</v>
@@ -9695,7 +9695,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L8" s="179">
-        <v>0.49589041095890413</v>
+        <v>0.50958904109589043</v>
       </c>
       <c r="M8" s="180">
         <v>0</v>
@@ -9724,15 +9724,15 @@
       <c r="U8" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V8" s="275"/>
-      <c r="W8" s="275"/>
+      <c r="V8" s="267"/>
+      <c r="W8" s="267"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" s="195">
-        <v>0.90848563416936845</v>
+        <v>0.90964135785836386</v>
       </c>
       <c r="B9" s="174">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="C9" s="176">
         <v>0</v>
@@ -9741,13 +9741,13 @@
         <v>1000000</v>
       </c>
       <c r="E9" s="174">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="F9" s="174">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="G9" s="175">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H9" s="177" t="str">
         <v>#N/A</v>
@@ -9762,7 +9762,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L9" s="179">
-        <v>0.50410958904109593</v>
+        <v>0.49041095890410957</v>
       </c>
       <c r="M9" s="180">
         <v>0</v>
@@ -9791,15 +9791,15 @@
       <c r="U9" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V9" s="275"/>
-      <c r="W9" s="275"/>
+      <c r="V9" s="267"/>
+      <c r="W9" s="267"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" s="195">
-        <v>0.89360865189861183</v>
+        <v>0.89499236140936644</v>
       </c>
       <c r="B10" s="174">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="C10" s="176">
         <v>0</v>
@@ -9808,13 +9808,13 @@
         <v>1000000</v>
       </c>
       <c r="E10" s="174">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="F10" s="174">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="G10" s="175">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H10" s="177" t="str">
         <v>#N/A</v>
@@ -9829,7 +9829,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L10" s="179">
-        <v>0.49589041095890413</v>
+        <v>0.50684931506849318</v>
       </c>
       <c r="M10" s="180">
         <v>0</v>
@@ -9858,15 +9858,15 @@
       <c r="U10" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V10" s="275"/>
-      <c r="W10" s="275"/>
+      <c r="V10" s="267"/>
+      <c r="W10" s="267"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" s="195">
-        <v>0.87810972118544339</v>
+        <v>0.8801545225635693</v>
       </c>
       <c r="B11" s="174">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="C11" s="176">
         <v>0</v>
@@ -9875,13 +9875,13 @@
         <v>1000000</v>
       </c>
       <c r="E11" s="174">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="F11" s="174">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="G11" s="175">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H11" s="177" t="str">
         <v>#N/A</v>
@@ -9896,7 +9896,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L11" s="179">
-        <v>0.50410958904109593</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M11" s="180">
         <v>0</v>
@@ -9925,15 +9925,15 @@
       <c r="U11" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V11" s="275"/>
-      <c r="W11" s="275"/>
+      <c r="V11" s="267"/>
+      <c r="W11" s="267"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" s="195">
-        <v>0.86258376609713372</v>
+        <v>0.86508701348992212</v>
       </c>
       <c r="B12" s="174">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="C12" s="176">
         <v>0</v>
@@ -9942,13 +9942,13 @@
         <v>1000000</v>
       </c>
       <c r="E12" s="174">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="F12" s="174">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="G12" s="175">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H12" s="177" t="str">
         <v>#N/A</v>
@@ -9963,7 +9963,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L12" s="179">
-        <v>0.49589041095890413</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M12" s="180">
         <v>0</v>
@@ -9992,15 +9992,15 @@
       <c r="U12" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V12" s="275"/>
-      <c r="W12" s="275"/>
+      <c r="V12" s="267"/>
+      <c r="W12" s="267"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" s="195">
-        <v>0.84638478006872575</v>
+        <v>0.84994849342450751</v>
       </c>
       <c r="B13" s="174">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="C13" s="176">
         <v>0</v>
@@ -10009,13 +10009,13 @@
         <v>1000000</v>
       </c>
       <c r="E13" s="174">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="F13" s="174">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="G13" s="175">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H13" s="177" t="str">
         <v>#N/A</v>
@@ -10030,7 +10030,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L13" s="179">
-        <v>0.50958904109589043</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M13" s="180">
         <v>0</v>
@@ -10059,15 +10059,15 @@
       <c r="U13" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V13" s="275"/>
-      <c r="W13" s="275"/>
+      <c r="V13" s="267"/>
+      <c r="W13" s="267"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" s="195">
-        <v>0.83012725902555851</v>
+        <v>0.83436437093232152</v>
       </c>
       <c r="B14" s="174">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="C14" s="176">
         <v>0</v>
@@ -10076,13 +10076,13 @@
         <v>1000000</v>
       </c>
       <c r="E14" s="174">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="F14" s="174">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="G14" s="175">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H14" s="177" t="str">
         <v>#N/A</v>
@@ -10097,7 +10097,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L14" s="179">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M14" s="180">
         <v>0</v>
@@ -10126,15 +10126,15 @@
       <c r="U14" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V14" s="275"/>
-      <c r="W14" s="275"/>
+      <c r="V14" s="267"/>
+      <c r="W14" s="267"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="195">
-        <v>0.8134325054127004</v>
+        <v>0.81864292987062703</v>
       </c>
       <c r="B15" s="174">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="C15" s="176">
         <v>0</v>
@@ -10143,13 +10143,13 @@
         <v>1000000</v>
       </c>
       <c r="E15" s="174">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="F15" s="174">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="G15" s="175">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H15" s="177" t="str">
         <v>#N/A</v>
@@ -10164,7 +10164,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L15" s="179">
-        <v>0.49863013698630138</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M15" s="180">
         <v>0</v>
@@ -10193,15 +10193,15 @@
       <c r="U15" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V15" s="275"/>
-      <c r="W15" s="275"/>
+      <c r="V15" s="267"/>
+      <c r="W15" s="267"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" s="195">
-        <v>0.79692238577986874</v>
+        <v>0.8027851993297439</v>
       </c>
       <c r="B16" s="174">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="C16" s="176">
         <v>0</v>
@@ -10210,13 +10210,13 @@
         <v>1000000</v>
       </c>
       <c r="E16" s="174">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="F16" s="174">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="G16" s="175">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H16" s="177" t="str">
         <v>#N/A</v>
@@ -10231,7 +10231,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L16" s="179">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M16" s="180">
         <v>0</v>
@@ -10260,15 +10260,15 @@
       <c r="U16" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V16" s="275"/>
-      <c r="W16" s="275"/>
+      <c r="V16" s="267"/>
+      <c r="W16" s="267"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="195">
-        <v>0.78102890658709501</v>
+        <v>0.78776177691322924</v>
       </c>
       <c r="B17" s="174">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="C17" s="176">
         <v>0</v>
@@ -10277,13 +10277,13 @@
         <v>1000000</v>
       </c>
       <c r="E17" s="174">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="F17" s="174">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="G17" s="175">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H17" s="177" t="str">
         <v>#N/A</v>
@@ -10298,7 +10298,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L17" s="179">
-        <v>0.50136986301369868</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M17" s="180">
         <v>0</v>
@@ -10327,15 +10327,15 @@
       <c r="U17" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V17" s="275"/>
-      <c r="W17" s="275"/>
+      <c r="V17" s="267"/>
+      <c r="W17" s="267"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="195">
-        <v>0.76564045846940665</v>
+        <v>0.77279849713683268</v>
       </c>
       <c r="B18" s="174">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="C18" s="176">
         <v>0</v>
@@ -10344,13 +10344,13 @@
         <v>1000000</v>
       </c>
       <c r="E18" s="174">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="F18" s="174">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="G18" s="175">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H18" s="177" t="str">
         <v>#N/A</v>
@@ -10365,7 +10365,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L18" s="179">
-        <v>0.49589041095890413</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M18" s="180">
         <v>0</v>
@@ -10394,15 +10394,15 @@
       <c r="U18" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V18" s="275"/>
-      <c r="W18" s="275"/>
+      <c r="V18" s="267"/>
+      <c r="W18" s="267"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="195">
-        <v>0.74986498717119976</v>
+        <v>0.75802071135131288</v>
       </c>
       <c r="B19" s="174">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="C19" s="176">
         <v>0</v>
@@ -10411,13 +10411,13 @@
         <v>1000000</v>
       </c>
       <c r="E19" s="174">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="F19" s="174">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="G19" s="175">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H19" s="177" t="str">
         <v>#N/A</v>
@@ -10432,7 +10432,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L19" s="179">
-        <v>0.50410958904109593</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M19" s="180">
         <v>0</v>
@@ -10461,15 +10461,15 @@
       <c r="U19" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V19" s="275"/>
-      <c r="W19" s="275"/>
+      <c r="V19" s="267"/>
+      <c r="W19" s="267"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="195">
-        <v>0.73411965313311145</v>
+        <v>0.74267176168050963</v>
       </c>
       <c r="B20" s="174">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="C20" s="176">
         <v>0</v>
@@ -10478,13 +10478,13 @@
         <v>1000000</v>
       </c>
       <c r="E20" s="174">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="F20" s="174">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="G20" s="175">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H20" s="177" t="str">
         <v>#N/A</v>
@@ -10499,7 +10499,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L20" s="179">
-        <v>0.49589041095890413</v>
+        <v>0.50958904109589043</v>
       </c>
       <c r="M20" s="180">
         <v>0</v>
@@ -10528,15 +10528,15 @@
       <c r="U20" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V20" s="275"/>
-      <c r="W20" s="275"/>
+      <c r="V20" s="267"/>
+      <c r="W20" s="267"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="195">
-        <v>0.71794182972811249</v>
+        <v>0.72750438324808642</v>
       </c>
       <c r="B21" s="174">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="C21" s="176">
         <v>0</v>
@@ -10545,13 +10545,13 @@
         <v>1000000</v>
       </c>
       <c r="E21" s="174">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="F21" s="174">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="G21" s="175">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H21" s="177" t="str">
         <v>#N/A</v>
@@ -10566,7 +10566,7 @@
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L21" s="179">
-        <v>0.50410958904109593</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M21" s="180">
         <v>0</v>
@@ -10595,15 +10595,15 @@
       <c r="U21" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V21" s="275"/>
-      <c r="W21" s="275"/>
+      <c r="V21" s="267"/>
+      <c r="W21" s="267"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="195">
-        <v>0.70208555969117814</v>
+        <v>0.71237079582453067</v>
       </c>
       <c r="B22" s="174">
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="C22" s="176">
         <v>0</v>
@@ -10612,10 +10612,10 @@
         <v>1000000</v>
       </c>
       <c r="E22" s="174">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="F22" s="174">
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="G22" s="175">
         <v>182</v>
@@ -10662,8 +10662,8 @@
       <c r="U22" s="196" t="str">
         <v>#N/A</v>
       </c>
-      <c r="V22" s="275"/>
-      <c r="W22" s="275"/>
+      <c r="V22" s="267"/>
+      <c r="W22" s="267"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="195" t="e">
@@ -10729,8 +10729,8 @@
       <c r="U23" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V23" s="275"/>
-      <c r="W23" s="275"/>
+      <c r="V23" s="267"/>
+      <c r="W23" s="267"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="195" t="e">
@@ -10796,8 +10796,8 @@
       <c r="U24" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V24" s="275"/>
-      <c r="W24" s="275"/>
+      <c r="V24" s="267"/>
+      <c r="W24" s="267"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="195" t="e">
@@ -10863,8 +10863,8 @@
       <c r="U25" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V25" s="275"/>
-      <c r="W25" s="275"/>
+      <c r="V25" s="267"/>
+      <c r="W25" s="267"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="195" t="e">
@@ -10930,8 +10930,8 @@
       <c r="U26" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V26" s="275"/>
-      <c r="W26" s="275"/>
+      <c r="V26" s="267"/>
+      <c r="W26" s="267"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="195" t="e">
@@ -10997,8 +10997,8 @@
       <c r="U27" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V27" s="275"/>
-      <c r="W27" s="275"/>
+      <c r="V27" s="267"/>
+      <c r="W27" s="267"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="195" t="e">
@@ -11064,8 +11064,8 @@
       <c r="U28" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V28" s="275"/>
-      <c r="W28" s="275"/>
+      <c r="V28" s="267"/>
+      <c r="W28" s="267"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="195" t="e">
@@ -11131,8 +11131,8 @@
       <c r="U29" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V29" s="275"/>
-      <c r="W29" s="275"/>
+      <c r="V29" s="267"/>
+      <c r="W29" s="267"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A30" s="195" t="e">
@@ -11198,8 +11198,8 @@
       <c r="U30" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V30" s="275"/>
-      <c r="W30" s="275"/>
+      <c r="V30" s="267"/>
+      <c r="W30" s="267"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A31" s="195" t="e">
@@ -11265,8 +11265,8 @@
       <c r="U31" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V31" s="275"/>
-      <c r="W31" s="275"/>
+      <c r="V31" s="267"/>
+      <c r="W31" s="267"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="195" t="e">
@@ -11332,8 +11332,8 @@
       <c r="U32" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V32" s="275"/>
-      <c r="W32" s="275"/>
+      <c r="V32" s="267"/>
+      <c r="W32" s="267"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A33" s="195" t="e">
@@ -11399,8 +11399,8 @@
       <c r="U33" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V33" s="275"/>
-      <c r="W33" s="275"/>
+      <c r="V33" s="267"/>
+      <c r="W33" s="267"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A34" s="195" t="e">
@@ -11466,8 +11466,8 @@
       <c r="U34" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V34" s="275"/>
-      <c r="W34" s="275"/>
+      <c r="V34" s="267"/>
+      <c r="W34" s="267"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A35" s="195" t="e">
@@ -11533,8 +11533,8 @@
       <c r="U35" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V35" s="275"/>
-      <c r="W35" s="275"/>
+      <c r="V35" s="267"/>
+      <c r="W35" s="267"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A36" s="195" t="e">
@@ -11600,8 +11600,8 @@
       <c r="U36" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V36" s="275"/>
-      <c r="W36" s="275"/>
+      <c r="V36" s="267"/>
+      <c r="W36" s="267"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A37" s="195" t="e">
@@ -11667,8 +11667,8 @@
       <c r="U37" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V37" s="275"/>
-      <c r="W37" s="275"/>
+      <c r="V37" s="267"/>
+      <c r="W37" s="267"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A38" s="195" t="e">
@@ -11734,8 +11734,8 @@
       <c r="U38" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V38" s="275"/>
-      <c r="W38" s="275"/>
+      <c r="V38" s="267"/>
+      <c r="W38" s="267"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A39" s="195" t="e">
@@ -11801,8 +11801,8 @@
       <c r="U39" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V39" s="275"/>
-      <c r="W39" s="275"/>
+      <c r="V39" s="267"/>
+      <c r="W39" s="267"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A40" s="195" t="e">
@@ -11868,8 +11868,8 @@
       <c r="U40" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V40" s="275"/>
-      <c r="W40" s="275"/>
+      <c r="V40" s="267"/>
+      <c r="W40" s="267"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A41" s="195" t="e">
@@ -11935,8 +11935,8 @@
       <c r="U41" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V41" s="275"/>
-      <c r="W41" s="275"/>
+      <c r="V41" s="267"/>
+      <c r="W41" s="267"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A42" s="195" t="e">
@@ -12002,8 +12002,8 @@
       <c r="U42" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V42" s="275"/>
-      <c r="W42" s="275"/>
+      <c r="V42" s="267"/>
+      <c r="W42" s="267"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A43" s="195" t="e">
@@ -12069,8 +12069,8 @@
       <c r="U43" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V43" s="275"/>
-      <c r="W43" s="275"/>
+      <c r="V43" s="267"/>
+      <c r="W43" s="267"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="195" t="e">
@@ -12136,8 +12136,8 @@
       <c r="U44" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V44" s="275"/>
-      <c r="W44" s="275"/>
+      <c r="V44" s="267"/>
+      <c r="W44" s="267"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="195" t="e">
@@ -12203,8 +12203,8 @@
       <c r="U45" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V45" s="275"/>
-      <c r="W45" s="275"/>
+      <c r="V45" s="267"/>
+      <c r="W45" s="267"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="195" t="e">
@@ -12270,8 +12270,8 @@
       <c r="U46" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V46" s="275"/>
-      <c r="W46" s="275"/>
+      <c r="V46" s="267"/>
+      <c r="W46" s="267"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="195" t="e">
@@ -12337,8 +12337,8 @@
       <c r="U47" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V47" s="275"/>
-      <c r="W47" s="275"/>
+      <c r="V47" s="267"/>
+      <c r="W47" s="267"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="195" t="e">
@@ -12404,8 +12404,8 @@
       <c r="U48" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V48" s="275"/>
-      <c r="W48" s="275"/>
+      <c r="V48" s="267"/>
+      <c r="W48" s="267"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="195" t="e">
@@ -12471,8 +12471,8 @@
       <c r="U49" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V49" s="275"/>
-      <c r="W49" s="275"/>
+      <c r="V49" s="267"/>
+      <c r="W49" s="267"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="195" t="e">
@@ -12538,8 +12538,8 @@
       <c r="U50" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V50" s="275"/>
-      <c r="W50" s="275"/>
+      <c r="V50" s="267"/>
+      <c r="W50" s="267"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="195" t="e">
@@ -12605,8 +12605,8 @@
       <c r="U51" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V51" s="275"/>
-      <c r="W51" s="275"/>
+      <c r="V51" s="267"/>
+      <c r="W51" s="267"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="195" t="e">
@@ -12672,8 +12672,8 @@
       <c r="U52" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V52" s="275"/>
-      <c r="W52" s="275"/>
+      <c r="V52" s="267"/>
+      <c r="W52" s="267"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="195" t="e">
@@ -12739,8 +12739,8 @@
       <c r="U53" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V53" s="275"/>
-      <c r="W53" s="275"/>
+      <c r="V53" s="267"/>
+      <c r="W53" s="267"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="195" t="e">
@@ -12806,8 +12806,8 @@
       <c r="U54" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V54" s="275"/>
-      <c r="W54" s="275"/>
+      <c r="V54" s="267"/>
+      <c r="W54" s="267"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="195" t="e">
@@ -12873,8 +12873,8 @@
       <c r="U55" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V55" s="275"/>
-      <c r="W55" s="275"/>
+      <c r="V55" s="267"/>
+      <c r="W55" s="267"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" s="195" t="e">
@@ -12940,8 +12940,8 @@
       <c r="U56" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V56" s="275"/>
-      <c r="W56" s="275"/>
+      <c r="V56" s="267"/>
+      <c r="W56" s="267"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="195" t="e">
@@ -13007,8 +13007,8 @@
       <c r="U57" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V57" s="275"/>
-      <c r="W57" s="275"/>
+      <c r="V57" s="267"/>
+      <c r="W57" s="267"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="195" t="e">
@@ -13074,8 +13074,8 @@
       <c r="U58" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V58" s="275"/>
-      <c r="W58" s="275"/>
+      <c r="V58" s="267"/>
+      <c r="W58" s="267"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="195" t="e">
@@ -13141,8 +13141,8 @@
       <c r="U59" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V59" s="275"/>
-      <c r="W59" s="275"/>
+      <c r="V59" s="267"/>
+      <c r="W59" s="267"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="195" t="e">
@@ -13208,8 +13208,8 @@
       <c r="U60" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V60" s="275"/>
-      <c r="W60" s="275"/>
+      <c r="V60" s="267"/>
+      <c r="W60" s="267"/>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" s="195" t="e">
@@ -13275,8 +13275,8 @@
       <c r="U61" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V61" s="275"/>
-      <c r="W61" s="275"/>
+      <c r="V61" s="267"/>
+      <c r="W61" s="267"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" s="195" t="e">
@@ -13342,8 +13342,8 @@
       <c r="U62" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V62" s="275"/>
-      <c r="W62" s="275"/>
+      <c r="V62" s="267"/>
+      <c r="W62" s="267"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" s="195" t="e">
@@ -13409,8 +13409,8 @@
       <c r="U63" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V63" s="275"/>
-      <c r="W63" s="275"/>
+      <c r="V63" s="267"/>
+      <c r="W63" s="267"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" s="195" t="e">
@@ -13476,8 +13476,8 @@
       <c r="U64" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V64" s="275"/>
-      <c r="W64" s="275"/>
+      <c r="V64" s="267"/>
+      <c r="W64" s="267"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65" s="195" t="e">
@@ -13543,8 +13543,8 @@
       <c r="U65" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V65" s="275"/>
-      <c r="W65" s="275"/>
+      <c r="V65" s="267"/>
+      <c r="W65" s="267"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66" s="195" t="e">
@@ -13610,8 +13610,8 @@
       <c r="U66" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V66" s="275"/>
-      <c r="W66" s="275"/>
+      <c r="V66" s="267"/>
+      <c r="W66" s="267"/>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67" s="195" t="e">
@@ -13677,8 +13677,8 @@
       <c r="U67" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V67" s="275"/>
-      <c r="W67" s="275"/>
+      <c r="V67" s="267"/>
+      <c r="W67" s="267"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68" s="195" t="e">
@@ -13744,8 +13744,8 @@
       <c r="U68" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V68" s="275"/>
-      <c r="W68" s="275"/>
+      <c r="V68" s="267"/>
+      <c r="W68" s="267"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69" s="195" t="e">
@@ -13811,8 +13811,8 @@
       <c r="U69" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V69" s="275"/>
-      <c r="W69" s="275"/>
+      <c r="V69" s="267"/>
+      <c r="W69" s="267"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70" s="195" t="e">
@@ -13878,8 +13878,8 @@
       <c r="U70" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V70" s="275"/>
-      <c r="W70" s="275"/>
+      <c r="V70" s="267"/>
+      <c r="W70" s="267"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71" s="195" t="e">
@@ -13945,8 +13945,8 @@
       <c r="U71" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V71" s="275"/>
-      <c r="W71" s="275"/>
+      <c r="V71" s="267"/>
+      <c r="W71" s="267"/>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" s="195" t="e">
@@ -14012,8 +14012,8 @@
       <c r="U72" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V72" s="275"/>
-      <c r="W72" s="275"/>
+      <c r="V72" s="267"/>
+      <c r="W72" s="267"/>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73" s="195" t="e">
@@ -14079,8 +14079,8 @@
       <c r="U73" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V73" s="275"/>
-      <c r="W73" s="275"/>
+      <c r="V73" s="267"/>
+      <c r="W73" s="267"/>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74" s="195" t="e">
@@ -14146,8 +14146,8 @@
       <c r="U74" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V74" s="275"/>
-      <c r="W74" s="275"/>
+      <c r="V74" s="267"/>
+      <c r="W74" s="267"/>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75" s="195" t="e">
@@ -14213,8 +14213,8 @@
       <c r="U75" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V75" s="275"/>
-      <c r="W75" s="275"/>
+      <c r="V75" s="267"/>
+      <c r="W75" s="267"/>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76" s="195" t="e">
@@ -14280,8 +14280,8 @@
       <c r="U76" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V76" s="275"/>
-      <c r="W76" s="275"/>
+      <c r="V76" s="267"/>
+      <c r="W76" s="267"/>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77" s="195" t="e">
@@ -14347,8 +14347,8 @@
       <c r="U77" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V77" s="275"/>
-      <c r="W77" s="275"/>
+      <c r="V77" s="267"/>
+      <c r="W77" s="267"/>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78" s="195" t="e">
@@ -14414,8 +14414,8 @@
       <c r="U78" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V78" s="275"/>
-      <c r="W78" s="275"/>
+      <c r="V78" s="267"/>
+      <c r="W78" s="267"/>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79" s="195" t="e">
@@ -14481,8 +14481,8 @@
       <c r="U79" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V79" s="275"/>
-      <c r="W79" s="275"/>
+      <c r="V79" s="267"/>
+      <c r="W79" s="267"/>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A80" s="195" t="e">
@@ -14548,8 +14548,8 @@
       <c r="U80" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V80" s="275"/>
-      <c r="W80" s="275"/>
+      <c r="V80" s="267"/>
+      <c r="W80" s="267"/>
     </row>
     <row r="81" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A81" s="195" t="e">
@@ -14615,8 +14615,8 @@
       <c r="U81" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V81" s="275"/>
-      <c r="W81" s="275"/>
+      <c r="V81" s="267"/>
+      <c r="W81" s="267"/>
     </row>
     <row r="82" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A82" s="195" t="e">
@@ -14682,8 +14682,8 @@
       <c r="U82" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V82" s="275"/>
-      <c r="W82" s="275"/>
+      <c r="V82" s="267"/>
+      <c r="W82" s="267"/>
     </row>
     <row r="83" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A83" s="195" t="e">
@@ -14749,8 +14749,8 @@
       <c r="U83" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V83" s="275"/>
-      <c r="W83" s="275"/>
+      <c r="V83" s="267"/>
+      <c r="W83" s="267"/>
     </row>
     <row r="84" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A84" s="195" t="e">
@@ -14816,8 +14816,8 @@
       <c r="U84" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V84" s="275"/>
-      <c r="W84" s="275"/>
+      <c r="V84" s="267"/>
+      <c r="W84" s="267"/>
     </row>
     <row r="85" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A85" s="195" t="e">
@@ -14883,8 +14883,8 @@
       <c r="U85" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V85" s="275"/>
-      <c r="W85" s="275"/>
+      <c r="V85" s="267"/>
+      <c r="W85" s="267"/>
     </row>
     <row r="86" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A86" s="195" t="e">
@@ -14950,8 +14950,8 @@
       <c r="U86" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V86" s="275"/>
-      <c r="W86" s="275"/>
+      <c r="V86" s="267"/>
+      <c r="W86" s="267"/>
     </row>
     <row r="87" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A87" s="195" t="e">
@@ -15017,8 +15017,8 @@
       <c r="U87" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V87" s="275"/>
-      <c r="W87" s="275"/>
+      <c r="V87" s="267"/>
+      <c r="W87" s="267"/>
     </row>
     <row r="88" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A88" s="195" t="e">
@@ -15084,8 +15084,8 @@
       <c r="U88" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V88" s="275"/>
-      <c r="W88" s="275"/>
+      <c r="V88" s="267"/>
+      <c r="W88" s="267"/>
     </row>
     <row r="89" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A89" s="195" t="e">
@@ -15151,8 +15151,8 @@
       <c r="U89" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V89" s="275"/>
-      <c r="W89" s="275"/>
+      <c r="V89" s="267"/>
+      <c r="W89" s="267"/>
     </row>
     <row r="90" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A90" s="195" t="e">
@@ -15218,8 +15218,8 @@
       <c r="U90" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V90" s="275"/>
-      <c r="W90" s="275"/>
+      <c r="V90" s="267"/>
+      <c r="W90" s="267"/>
     </row>
     <row r="91" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A91" s="195" t="e">
@@ -15285,8 +15285,8 @@
       <c r="U91" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V91" s="275"/>
-      <c r="W91" s="275"/>
+      <c r="V91" s="267"/>
+      <c r="W91" s="267"/>
     </row>
     <row r="92" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A92" s="195" t="e">
@@ -15352,8 +15352,8 @@
       <c r="U92" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V92" s="275"/>
-      <c r="W92" s="275"/>
+      <c r="V92" s="267"/>
+      <c r="W92" s="267"/>
     </row>
     <row r="93" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A93" s="195" t="e">
@@ -15419,8 +15419,8 @@
       <c r="U93" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V93" s="275"/>
-      <c r="W93" s="275"/>
+      <c r="V93" s="267"/>
+      <c r="W93" s="267"/>
     </row>
     <row r="94" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A94" s="195" t="e">
@@ -15486,8 +15486,8 @@
       <c r="U94" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V94" s="275"/>
-      <c r="W94" s="275"/>
+      <c r="V94" s="267"/>
+      <c r="W94" s="267"/>
     </row>
     <row r="95" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A95" s="195" t="e">
@@ -15553,8 +15553,8 @@
       <c r="U95" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V95" s="275"/>
-      <c r="W95" s="275"/>
+      <c r="V95" s="267"/>
+      <c r="W95" s="267"/>
     </row>
     <row r="96" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A96" s="195" t="e">
@@ -15620,8 +15620,8 @@
       <c r="U96" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V96" s="275"/>
-      <c r="W96" s="275"/>
+      <c r="V96" s="267"/>
+      <c r="W96" s="267"/>
     </row>
     <row r="97" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A97" s="195" t="e">
@@ -15687,8 +15687,8 @@
       <c r="U97" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V97" s="275"/>
-      <c r="W97" s="275"/>
+      <c r="V97" s="267"/>
+      <c r="W97" s="267"/>
     </row>
     <row r="98" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A98" s="195" t="e">
@@ -15754,8 +15754,8 @@
       <c r="U98" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V98" s="275"/>
-      <c r="W98" s="275"/>
+      <c r="V98" s="267"/>
+      <c r="W98" s="267"/>
     </row>
     <row r="99" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A99" s="195" t="e">
@@ -15821,8 +15821,8 @@
       <c r="U99" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V99" s="275"/>
-      <c r="W99" s="275"/>
+      <c r="V99" s="267"/>
+      <c r="W99" s="267"/>
     </row>
     <row r="100" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A100" s="195" t="e">
@@ -15888,8 +15888,8 @@
       <c r="U100" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V100" s="275"/>
-      <c r="W100" s="275"/>
+      <c r="V100" s="267"/>
+      <c r="W100" s="267"/>
     </row>
     <row r="101" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A101" s="195" t="e">
@@ -15955,8 +15955,8 @@
       <c r="U101" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V101" s="275"/>
-      <c r="W101" s="275"/>
+      <c r="V101" s="267"/>
+      <c r="W101" s="267"/>
     </row>
     <row r="102" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A102" s="195" t="e">
@@ -16022,8 +16022,8 @@
       <c r="U102" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V102" s="275"/>
-      <c r="W102" s="275"/>
+      <c r="V102" s="267"/>
+      <c r="W102" s="267"/>
     </row>
     <row r="103" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A103" s="195" t="e">
@@ -16089,8 +16089,8 @@
       <c r="U103" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V103" s="275"/>
-      <c r="W103" s="275"/>
+      <c r="V103" s="267"/>
+      <c r="W103" s="267"/>
     </row>
     <row r="104" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A104" s="195" t="e">
@@ -16156,8 +16156,8 @@
       <c r="U104" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V104" s="275"/>
-      <c r="W104" s="275"/>
+      <c r="V104" s="267"/>
+      <c r="W104" s="267"/>
     </row>
     <row r="105" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A105" s="195" t="e">
@@ -16223,8 +16223,8 @@
       <c r="U105" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V105" s="275"/>
-      <c r="W105" s="275"/>
+      <c r="V105" s="267"/>
+      <c r="W105" s="267"/>
     </row>
     <row r="106" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A106" s="195" t="e">
@@ -16290,8 +16290,8 @@
       <c r="U106" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V106" s="275"/>
-      <c r="W106" s="275"/>
+      <c r="V106" s="267"/>
+      <c r="W106" s="267"/>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A107" s="195" t="e">
@@ -16357,8 +16357,8 @@
       <c r="U107" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V107" s="275"/>
-      <c r="W107" s="275"/>
+      <c r="V107" s="267"/>
+      <c r="W107" s="267"/>
     </row>
     <row r="108" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A108" s="195" t="e">
@@ -16424,8 +16424,8 @@
       <c r="U108" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V108" s="275"/>
-      <c r="W108" s="275"/>
+      <c r="V108" s="267"/>
+      <c r="W108" s="267"/>
     </row>
     <row r="109" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A109" s="195" t="e">
@@ -16491,8 +16491,8 @@
       <c r="U109" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V109" s="275"/>
-      <c r="W109" s="275"/>
+      <c r="V109" s="267"/>
+      <c r="W109" s="267"/>
     </row>
     <row r="110" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A110" s="195" t="e">
@@ -16558,8 +16558,8 @@
       <c r="U110" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V110" s="275"/>
-      <c r="W110" s="275"/>
+      <c r="V110" s="267"/>
+      <c r="W110" s="267"/>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A111" s="195" t="e">
@@ -16625,8 +16625,8 @@
       <c r="U111" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V111" s="275"/>
-      <c r="W111" s="275"/>
+      <c r="V111" s="267"/>
+      <c r="W111" s="267"/>
     </row>
     <row r="112" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A112" s="195" t="e">
@@ -16692,8 +16692,8 @@
       <c r="U112" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V112" s="275"/>
-      <c r="W112" s="275"/>
+      <c r="V112" s="267"/>
+      <c r="W112" s="267"/>
     </row>
     <row r="113" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A113" s="195" t="e">
@@ -16759,8 +16759,8 @@
       <c r="U113" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V113" s="275"/>
-      <c r="W113" s="275"/>
+      <c r="V113" s="267"/>
+      <c r="W113" s="267"/>
     </row>
     <row r="114" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A114" s="195" t="e">
@@ -16826,8 +16826,8 @@
       <c r="U114" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V114" s="275"/>
-      <c r="W114" s="275"/>
+      <c r="V114" s="267"/>
+      <c r="W114" s="267"/>
     </row>
     <row r="115" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A115" s="195" t="e">
@@ -16893,8 +16893,8 @@
       <c r="U115" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V115" s="275"/>
-      <c r="W115" s="275"/>
+      <c r="V115" s="267"/>
+      <c r="W115" s="267"/>
     </row>
     <row r="116" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A116" s="195" t="e">
@@ -16960,8 +16960,8 @@
       <c r="U116" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V116" s="275"/>
-      <c r="W116" s="275"/>
+      <c r="V116" s="267"/>
+      <c r="W116" s="267"/>
     </row>
     <row r="117" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A117" s="195" t="e">
@@ -17027,8 +17027,8 @@
       <c r="U117" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V117" s="275"/>
-      <c r="W117" s="275"/>
+      <c r="V117" s="267"/>
+      <c r="W117" s="267"/>
     </row>
     <row r="118" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A118" s="195" t="e">
@@ -17094,8 +17094,8 @@
       <c r="U118" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V118" s="275"/>
-      <c r="W118" s="275"/>
+      <c r="V118" s="267"/>
+      <c r="W118" s="267"/>
     </row>
     <row r="119" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A119" s="195" t="e">
@@ -17161,8 +17161,8 @@
       <c r="U119" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V119" s="275"/>
-      <c r="W119" s="275"/>
+      <c r="V119" s="267"/>
+      <c r="W119" s="267"/>
     </row>
     <row r="120" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A120" s="195" t="e">
@@ -17228,8 +17228,8 @@
       <c r="U120" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V120" s="275"/>
-      <c r="W120" s="275"/>
+      <c r="V120" s="267"/>
+      <c r="W120" s="267"/>
     </row>
     <row r="121" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A121" s="195" t="e">
@@ -17295,8 +17295,8 @@
       <c r="U121" s="196" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V121" s="275"/>
-      <c r="W121" s="275"/>
+      <c r="V121" s="267"/>
+      <c r="W121" s="267"/>
     </row>
     <row r="122" spans="1:23" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A122" s="197" t="e">
@@ -17362,8 +17362,8 @@
       <c r="U122" s="206" t="e">
         <v>#N/A</v>
       </c>
-      <c r="V122" s="275"/>
-      <c r="W122" s="275"/>
+      <c r="V122" s="267"/>
+      <c r="W122" s="267"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -17398,7 +17398,7 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="35" t="str">
         <f>Pricing!$G$14</f>
-        <v>obj_00940#0005</v>
+        <v>obj_003fa#0001</v>
       </c>
       <c r="C1" s="34" t="str">
         <f>UPPER(Pricing!$G$18)</f>
@@ -17455,7 +17455,7 @@
       </c>
       <c r="B4" s="41">
         <f t="array" ref="B4:B123">_xll.qlScheduleDates(Schedule)</f>
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="C4" s="43">
         <f t="array" ref="C4:C123">IF(Type="MIRROR",E4:E123,IF(Type="CUSTOM",F4:F123,IF(Type="STEP",G4:G123,IF(Type="FRENCH",H4:H123,D4:D123))))</f>
@@ -17491,7 +17491,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="41">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="C5" s="43">
         <v>1000000</v>
@@ -17525,7 +17525,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="41">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="C6" s="43">
         <v>1000000</v>
@@ -17559,7 +17559,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="41">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="C7" s="43">
         <v>1000000</v>
@@ -17593,7 +17593,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="41">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="C8" s="43">
         <v>1000000</v>
@@ -17627,7 +17627,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="41">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="C9" s="43">
         <v>1000000</v>
@@ -17661,7 +17661,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="41">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="C10" s="43">
         <v>1000000</v>
@@ -17695,7 +17695,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="41">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="C11" s="43">
         <v>1000000</v>
@@ -17729,7 +17729,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="41">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="C12" s="43">
         <v>1000000</v>
@@ -17763,7 +17763,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="41">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="C13" s="43">
         <v>1000000</v>
@@ -17797,7 +17797,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="41">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="C14" s="43">
         <v>1000000</v>
@@ -17831,7 +17831,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="41">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="C15" s="43">
         <v>1000000</v>
@@ -17865,7 +17865,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="41">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="C16" s="43">
         <v>1000000</v>
@@ -17899,7 +17899,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="41">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="C17" s="43">
         <v>1000000</v>
@@ -17933,7 +17933,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="41">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="C18" s="43">
         <v>1000000</v>
@@ -17967,7 +17967,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="41">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="C19" s="43">
         <v>1000000</v>
@@ -18001,7 +18001,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="41">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="C20" s="43">
         <v>1000000</v>
@@ -18035,7 +18035,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="41">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="C21" s="43">
         <v>1000000</v>
@@ -18069,7 +18069,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="41">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="C22" s="43">
         <v>1000000</v>
@@ -18103,7 +18103,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="41">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="C23" s="43">
         <v>1000000</v>
@@ -18137,7 +18137,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="41">
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="C24" s="43" t="e">
         <v>#N/A</v>
@@ -21572,29 +21572,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="272" t="s">
+      <c r="A1" s="273" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="273"/>
-      <c r="C1" s="273"/>
-      <c r="D1" s="273"/>
-      <c r="E1" s="273"/>
-      <c r="F1" s="273"/>
-      <c r="G1" s="273"/>
-      <c r="H1" s="273"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="273"/>
-      <c r="L1" s="273"/>
-      <c r="M1" s="273"/>
-      <c r="N1" s="273"/>
-      <c r="O1" s="273"/>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="273"/>
-      <c r="R1" s="273"/>
-      <c r="S1" s="273"/>
-      <c r="T1" s="273"/>
-      <c r="U1" s="274"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="274"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="274"/>
+      <c r="L1" s="274"/>
+      <c r="M1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="274"/>
+      <c r="R1" s="274"/>
+      <c r="S1" s="274"/>
+      <c r="T1" s="274"/>
+      <c r="U1" s="275"/>
     </row>
     <row r="2" spans="1:40" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="221" t="s">
@@ -21665,25 +21665,25 @@
     <row r="3" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="224">
         <f t="array" ref="A3:A122">_xll.qlYieldTSDiscount(DiscountCurve,_xll.ohPack(B3:B122))</f>
-        <v>0.98762977471753821</v>
+        <v>0.98781996868675226</v>
       </c>
       <c r="B3" s="225">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="C3" s="226">
-        <v>13809.440249901381</v>
+        <v>13511.213627523277</v>
       </c>
       <c r="D3" s="226">
         <v>1000000</v>
       </c>
       <c r="E3" s="225">
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="F3" s="225">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="G3" s="227">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H3" s="228" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21692,16 +21692,16 @@
         <v>0</v>
       </c>
       <c r="J3" s="225">
-        <v>41859</v>
+        <v>41884</v>
       </c>
       <c r="K3" s="227" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L3" s="230">
-        <v>0.50684931506849318</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M3" s="231">
-        <v>2.7245652384940564E-2</v>
+        <v>2.7246370022353569E-2</v>
       </c>
       <c r="N3" s="231" t="str">
         <v>#N/A</v>
@@ -21710,10 +21710,10 @@
         <v>1</v>
       </c>
       <c r="P3" s="231">
-        <v>2.7245652384940568E-2</v>
+        <v>2.7246370022353569E-2</v>
       </c>
       <c r="Q3" s="231">
-        <v>-3.4694469519536142E-18</v>
+        <v>0</v>
       </c>
       <c r="R3" s="231">
         <v>0</v>
@@ -21749,25 +21749,25 @@
     </row>
     <row r="4" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="236">
-        <v>0.97593905629035904</v>
+        <v>0.97589522175637922</v>
       </c>
       <c r="B4" s="237">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="C4" s="238">
-        <v>12657.253290132787</v>
+        <v>13024.751506146125</v>
       </c>
       <c r="D4" s="238">
         <v>1000000</v>
       </c>
       <c r="E4" s="237">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="F4" s="237">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="G4" s="239">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H4" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21776,16 +21776,16 @@
         <v>0</v>
       </c>
       <c r="J4" s="237">
-        <v>42044</v>
+        <v>42065</v>
       </c>
       <c r="K4" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L4" s="242">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M4" s="243">
-        <v>2.5384051928013553E-2</v>
+        <v>2.5837142933387694E-2</v>
       </c>
       <c r="N4" s="243" t="str">
         <v>#N/A</v>
@@ -21794,7 +21794,7 @@
         <v>1</v>
       </c>
       <c r="P4" s="243">
-        <v>2.5384051928013553E-2</v>
+        <v>2.5837142933387694E-2</v>
       </c>
       <c r="Q4" s="243">
         <v>0</v>
@@ -21833,22 +21833,22 @@
     </row>
     <row r="5" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="236">
-        <v>0.963823130511412</v>
+        <v>0.96381080870229641</v>
       </c>
       <c r="B5" s="237">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="C5" s="238">
-        <v>13718.338166651467</v>
+        <v>13796.456181262018</v>
       </c>
       <c r="D5" s="238">
         <v>1000000</v>
       </c>
       <c r="E5" s="237">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="F5" s="237">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="G5" s="239">
         <v>182</v>
@@ -21860,7 +21860,7 @@
         <v>0</v>
       </c>
       <c r="J5" s="237">
-        <v>42226</v>
+        <v>42249</v>
       </c>
       <c r="K5" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
@@ -21869,7 +21869,7 @@
         <v>0.49863013698630138</v>
       </c>
       <c r="M5" s="243">
-        <v>2.7512051817735084E-2</v>
+        <v>2.7668717066816683E-2</v>
       </c>
       <c r="N5" s="243" t="str">
         <v>#N/A</v>
@@ -21878,7 +21878,7 @@
         <v>1</v>
       </c>
       <c r="P5" s="243">
-        <v>2.7512051817735084E-2</v>
+        <v>2.7668717066816683E-2</v>
       </c>
       <c r="Q5" s="243">
         <v>0</v>
@@ -21917,25 +21917,25 @@
     </row>
     <row r="6" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="236">
-        <v>0.95091964847149946</v>
+        <v>0.95092413549530208</v>
       </c>
       <c r="B6" s="237">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="C6" s="238">
-        <v>14974.528801630973</v>
+        <v>15049.178783807181</v>
       </c>
       <c r="D6" s="238">
         <v>1000000</v>
       </c>
       <c r="E6" s="237">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="F6" s="237">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="G6" s="239">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H6" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -21944,16 +21944,16 @@
         <v>0</v>
       </c>
       <c r="J6" s="237">
-        <v>42408</v>
+        <v>42431</v>
       </c>
       <c r="K6" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L6" s="242">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M6" s="243">
-        <v>3.0031335234040137E-2</v>
+        <v>2.9852990522226203E-2</v>
       </c>
       <c r="N6" s="243" t="str">
         <v>#N/A</v>
@@ -21962,10 +21962,10 @@
         <v>1</v>
       </c>
       <c r="P6" s="243">
-        <v>3.0031335234040134E-2</v>
+        <v>2.9852990522226203E-2</v>
       </c>
       <c r="Q6" s="243">
-        <v>3.4694469519536142E-18</v>
+        <v>0</v>
       </c>
       <c r="R6" s="243">
         <v>0</v>
@@ -22001,25 +22001,25 @@
     </row>
     <row r="7" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="236">
-        <v>0.9372080274699961</v>
+        <v>0.93760752950670501</v>
       </c>
       <c r="B7" s="237">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="C7" s="238">
-        <v>16041.97064241597</v>
+        <v>15588.562658565896</v>
       </c>
       <c r="D7" s="238">
         <v>1000000</v>
       </c>
       <c r="E7" s="237">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="F7" s="237">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="G7" s="239">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H7" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22028,16 +22028,16 @@
         <v>0</v>
       </c>
       <c r="J7" s="237">
-        <v>42590</v>
+        <v>42615</v>
       </c>
       <c r="K7" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L7" s="242">
-        <v>0.50410958904109593</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M7" s="243">
-        <v>3.1822387415662109E-2</v>
+        <v>3.1435499283848353E-2</v>
       </c>
       <c r="N7" s="243" t="str">
         <v>#N/A</v>
@@ -22046,7 +22046,7 @@
         <v>1</v>
       </c>
       <c r="P7" s="243">
-        <v>3.1822387415662109E-2</v>
+        <v>3.1435499283848353E-2</v>
       </c>
       <c r="Q7" s="243">
         <v>0</v>
@@ -22085,25 +22085,25 @@
     </row>
     <row r="8" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="236">
-        <v>0.92319139827288144</v>
+        <v>0.92348093763004924</v>
       </c>
       <c r="B8" s="237">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="C8" s="238">
-        <v>16712.855616306089</v>
+        <v>16851.249849254124</v>
       </c>
       <c r="D8" s="238">
         <v>1000000</v>
       </c>
       <c r="E8" s="237">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="F8" s="237">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="G8" s="239">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H8" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22112,16 +22112,16 @@
         <v>0</v>
       </c>
       <c r="J8" s="237">
-        <v>42774</v>
+        <v>42796</v>
       </c>
       <c r="K8" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L8" s="242">
-        <v>0.49589041095890413</v>
+        <v>0.50958904109589043</v>
       </c>
       <c r="M8" s="243">
-        <v>3.3702719889236031E-2</v>
+        <v>3.3068312876224491E-2</v>
       </c>
       <c r="N8" s="243" t="str">
         <v>#N/A</v>
@@ -22130,7 +22130,7 @@
         <v>1</v>
       </c>
       <c r="P8" s="243">
-        <v>3.3702719889236031E-2</v>
+        <v>3.3068312876224491E-2</v>
       </c>
       <c r="Q8" s="243">
         <v>0</v>
@@ -22169,25 +22169,25 @@
     </row>
     <row r="9" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="236">
-        <v>0.90848563416936845</v>
+        <v>0.90964135785836386</v>
       </c>
       <c r="B9" s="237">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="C9" s="238">
-        <v>18028.383932473524</v>
+        <v>17050.012579906015</v>
       </c>
       <c r="D9" s="238">
         <v>1000000</v>
       </c>
       <c r="E9" s="237">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="F9" s="237">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="G9" s="239">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="H9" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22196,16 +22196,16 @@
         <v>0</v>
       </c>
       <c r="J9" s="237">
-        <v>42955</v>
+        <v>42982</v>
       </c>
       <c r="K9" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L9" s="242">
-        <v>0.50410958904109593</v>
+        <v>0.49041095890410957</v>
       </c>
       <c r="M9" s="243">
-        <v>3.576282682256976E-2</v>
+        <v>3.4766785428299973E-2</v>
       </c>
       <c r="N9" s="243" t="str">
         <v>#N/A</v>
@@ -22214,7 +22214,7 @@
         <v>1</v>
       </c>
       <c r="P9" s="243">
-        <v>3.576282682256976E-2</v>
+        <v>3.4766785428299973E-2</v>
       </c>
       <c r="Q9" s="243">
         <v>0</v>
@@ -22253,25 +22253,25 @@
     </row>
     <row r="10" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="236">
-        <v>0.89360865189861183</v>
+        <v>0.89499236140936644</v>
       </c>
       <c r="B10" s="237">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="C10" s="238">
-        <v>18557.870922345512</v>
+        <v>18339.492015127409</v>
       </c>
       <c r="D10" s="238">
         <v>1000000</v>
       </c>
       <c r="E10" s="237">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="F10" s="237">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="G10" s="239">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="H10" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22280,16 +22280,16 @@
         <v>0</v>
       </c>
       <c r="J10" s="237">
-        <v>43139</v>
+        <v>43161</v>
       </c>
       <c r="K10" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L10" s="242">
-        <v>0.49589041095890413</v>
+        <v>0.50684931506849318</v>
       </c>
       <c r="M10" s="243">
-        <v>3.7423330865503382E-2</v>
+        <v>3.6183322083900023E-2</v>
       </c>
       <c r="N10" s="243" t="str">
         <v>#N/A</v>
@@ -22298,10 +22298,10 @@
         <v>1</v>
       </c>
       <c r="P10" s="243">
-        <v>3.7423330865503375E-2</v>
+        <v>3.618332208390003E-2</v>
       </c>
       <c r="Q10" s="243">
-        <v>6.9388939039072284E-18</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="R10" s="243">
         <v>0</v>
@@ -22337,25 +22337,25 @@
     </row>
     <row r="11" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="236">
-        <v>0.87810972118544339</v>
+        <v>0.8801545225635693</v>
       </c>
       <c r="B11" s="237">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="C11" s="238">
-        <v>19507.481768269889</v>
+        <v>18592.078960460109</v>
       </c>
       <c r="D11" s="238">
         <v>1000000</v>
       </c>
       <c r="E11" s="237">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="F11" s="237">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="G11" s="239">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H11" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22364,16 +22364,16 @@
         <v>0</v>
       </c>
       <c r="J11" s="237">
-        <v>43320</v>
+        <v>43346</v>
       </c>
       <c r="K11" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L11" s="242">
-        <v>0.50410958904109593</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M11" s="243">
-        <v>3.869690676857885E-2</v>
+        <v>3.7286312200922746E-2</v>
       </c>
       <c r="N11" s="243" t="str">
         <v>#N/A</v>
@@ -22382,10 +22382,10 @@
         <v>1</v>
       </c>
       <c r="P11" s="243">
-        <v>3.8696906768578843E-2</v>
+        <v>3.7286312200922753E-2</v>
       </c>
       <c r="Q11" s="243">
-        <v>6.9388939039072284E-18</v>
+        <v>-6.9388939039072284E-18</v>
       </c>
       <c r="R11" s="243">
         <v>0</v>
@@ -22421,25 +22421,25 @@
     </row>
     <row r="12" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="236">
-        <v>0.86258376609713372</v>
+        <v>0.86508701348992212</v>
       </c>
       <c r="B12" s="237">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="C12" s="238">
-        <v>19876.495884307398</v>
+        <v>19168.539832428389</v>
       </c>
       <c r="D12" s="238">
         <v>1000000</v>
       </c>
       <c r="E12" s="237">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="F12" s="237">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="G12" s="239">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H12" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22448,16 +22448,16 @@
         <v>0</v>
       </c>
       <c r="J12" s="237">
-        <v>43504</v>
+        <v>43528</v>
       </c>
       <c r="K12" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L12" s="242">
-        <v>0.49589041095890413</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M12" s="243">
-        <v>4.0082436451780112E-2</v>
+        <v>3.8442401312287704E-2</v>
       </c>
       <c r="N12" s="243" t="str">
         <v>#N/A</v>
@@ -22466,7 +22466,7 @@
         <v>1</v>
       </c>
       <c r="P12" s="243">
-        <v>4.0082436451780112E-2</v>
+        <v>3.8442401312287704E-2</v>
       </c>
       <c r="Q12" s="243">
         <v>0</v>
@@ -22505,25 +22505,25 @@
     </row>
     <row r="13" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="236">
-        <v>0.84638478006872575</v>
+        <v>0.84994849342450751</v>
       </c>
       <c r="B13" s="237">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="C13" s="238">
-        <v>21223.85904367641</v>
+        <v>19796.320094451981</v>
       </c>
       <c r="D13" s="238">
         <v>1000000</v>
       </c>
       <c r="E13" s="237">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="F13" s="237">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="G13" s="239">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H13" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22532,16 +22532,16 @@
         <v>0</v>
       </c>
       <c r="J13" s="237">
-        <v>43685</v>
+        <v>43710</v>
       </c>
       <c r="K13" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L13" s="242">
-        <v>0.50958904109589043</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M13" s="243">
-        <v>4.1648970703988653E-2</v>
+        <v>3.9701411178433912E-2</v>
       </c>
       <c r="N13" s="243" t="str">
         <v>#N/A</v>
@@ -22550,10 +22550,10 @@
         <v>1</v>
       </c>
       <c r="P13" s="243">
-        <v>4.1648970703988646E-2</v>
+        <v>3.9701411178433912E-2</v>
       </c>
       <c r="Q13" s="243">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R13" s="243">
         <v>0</v>
@@ -22589,25 +22589,25 @@
     </row>
     <row r="14" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="236">
-        <v>0.83012725902555851</v>
+        <v>0.83436437093232152</v>
       </c>
       <c r="B14" s="237">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="C14" s="238">
-        <v>21421.175088995657</v>
+        <v>20611.521200382122</v>
       </c>
       <c r="D14" s="238">
         <v>1000000</v>
       </c>
       <c r="E14" s="237">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="F14" s="237">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="G14" s="239">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H14" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22616,16 +22616,16 @@
         <v>0</v>
       </c>
       <c r="J14" s="237">
-        <v>43871</v>
+        <v>43892</v>
       </c>
       <c r="K14" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L14" s="242">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M14" s="243">
-        <v>4.2960048942216562E-2</v>
+        <v>4.0886984989888443E-2</v>
       </c>
       <c r="N14" s="243" t="str">
         <v>#N/A</v>
@@ -22634,10 +22634,10 @@
         <v>1</v>
       </c>
       <c r="P14" s="243">
-        <v>4.2960048942216569E-2</v>
+        <v>4.0886984989888443E-2</v>
       </c>
       <c r="Q14" s="243">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R14" s="243">
         <v>0</v>
@@ -22673,25 +22673,25 @@
     </row>
     <row r="15" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="236">
-        <v>0.8134325054127004</v>
+        <v>0.81864292987062703</v>
       </c>
       <c r="B15" s="237">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="C15" s="238">
-        <v>21929.382639711785</v>
+        <v>20769.908221588423</v>
       </c>
       <c r="D15" s="238">
         <v>1000000</v>
       </c>
       <c r="E15" s="237">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="F15" s="237">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="G15" s="239">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H15" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22700,16 +22700,16 @@
         <v>0</v>
       </c>
       <c r="J15" s="237">
-        <v>44053</v>
+        <v>44076</v>
       </c>
       <c r="K15" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L15" s="242">
-        <v>0.49863013698630138</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M15" s="243">
-        <v>4.3979256392828577E-2</v>
+        <v>4.1884069065634105E-2</v>
       </c>
       <c r="N15" s="243" t="str">
         <v>#N/A</v>
@@ -22718,7 +22718,7 @@
         <v>1</v>
       </c>
       <c r="P15" s="243">
-        <v>4.397925639282857E-2</v>
+        <v>4.1884069065634098E-2</v>
       </c>
       <c r="Q15" s="243">
         <v>6.9388939039072284E-18</v>
@@ -22757,25 +22757,25 @@
     </row>
     <row r="16" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="236">
-        <v>0.79692238577986874</v>
+        <v>0.8027851993297439</v>
       </c>
       <c r="B16" s="237">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="C16" s="238">
-        <v>22386.032939360146</v>
+        <v>21448.935496471309</v>
       </c>
       <c r="D16" s="238">
         <v>1000000</v>
       </c>
       <c r="E16" s="237">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="F16" s="237">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="G16" s="239">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H16" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22784,16 +22784,16 @@
         <v>0</v>
       </c>
       <c r="J16" s="237">
-        <v>44235</v>
+        <v>44257</v>
       </c>
       <c r="K16" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L16" s="242">
-        <v>0.49863013698630138</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M16" s="243">
-        <v>4.4895066059705786E-2</v>
+        <v>4.2548160088108848E-2</v>
       </c>
       <c r="N16" s="243" t="str">
         <v>#N/A</v>
@@ -22802,7 +22802,7 @@
         <v>1</v>
       </c>
       <c r="P16" s="243">
-        <v>4.4895066059705786E-2</v>
+        <v>4.2548160088108848E-2</v>
       </c>
       <c r="Q16" s="243">
         <v>0</v>
@@ -22841,25 +22841,25 @@
     </row>
     <row r="17" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="236">
-        <v>0.78102890658709501</v>
+        <v>0.78776177691322924</v>
       </c>
       <c r="B17" s="237">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="C17" s="238">
-        <v>22910.736153002319</v>
+        <v>21264.910434920293</v>
       </c>
       <c r="D17" s="238">
         <v>1000000</v>
       </c>
       <c r="E17" s="237">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="F17" s="237">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="G17" s="239">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H17" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22868,16 +22868,16 @@
         <v>0</v>
       </c>
       <c r="J17" s="237">
-        <v>44417</v>
+        <v>44441</v>
       </c>
       <c r="K17" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L17" s="242">
-        <v>0.50136986301369868</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M17" s="243">
-        <v>4.5696277026480034E-2</v>
+        <v>4.2882277948872408E-2</v>
       </c>
       <c r="N17" s="243" t="str">
         <v>#N/A</v>
@@ -22886,7 +22886,7 @@
         <v>1</v>
       </c>
       <c r="P17" s="243">
-        <v>4.5696277026480034E-2</v>
+        <v>4.2882277948872408E-2</v>
       </c>
       <c r="Q17" s="243">
         <v>0</v>
@@ -22925,25 +22925,25 @@
     </row>
     <row r="18" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="236">
-        <v>0.76564045846940665</v>
+        <v>0.77279849713683268</v>
       </c>
       <c r="B18" s="237">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="C18" s="238">
-        <v>22872.341525955962</v>
+        <v>21785.457104138262</v>
       </c>
       <c r="D18" s="238">
         <v>1000000</v>
       </c>
       <c r="E18" s="237">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="F18" s="237">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="G18" s="239">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H18" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -22952,16 +22952,16 @@
         <v>0</v>
       </c>
       <c r="J18" s="237">
-        <v>44600</v>
+        <v>44622</v>
       </c>
       <c r="K18" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L18" s="242">
-        <v>0.49589041095890413</v>
+        <v>0.50410958904109593</v>
       </c>
       <c r="M18" s="243">
-        <v>4.6123782635215063E-2</v>
+        <v>4.321571653810035E-2</v>
       </c>
       <c r="N18" s="243" t="str">
         <v>#N/A</v>
@@ -22970,7 +22970,7 @@
         <v>1</v>
       </c>
       <c r="P18" s="243">
-        <v>4.6123782635215063E-2</v>
+        <v>4.321571653810035E-2</v>
       </c>
       <c r="Q18" s="243">
         <v>0</v>
@@ -23009,25 +23009,25 @@
     </row>
     <row r="19" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="236">
-        <v>0.74986498717119976</v>
+        <v>0.75802071135131288</v>
       </c>
       <c r="B19" s="237">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="C19" s="238">
-        <v>23335.466336405156</v>
+        <v>21632.492029286743</v>
       </c>
       <c r="D19" s="238">
         <v>1000000</v>
       </c>
       <c r="E19" s="237">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="F19" s="237">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="G19" s="239">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="H19" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -23036,16 +23036,16 @@
         <v>0</v>
       </c>
       <c r="J19" s="237">
-        <v>44781</v>
+        <v>44806</v>
       </c>
       <c r="K19" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L19" s="242">
-        <v>0.50410958904109593</v>
+        <v>0.49589041095890413</v>
       </c>
       <c r="M19" s="243">
-        <v>4.6290463112977617E-2</v>
+        <v>4.3623533650219121E-2</v>
       </c>
       <c r="N19" s="243" t="str">
         <v>#N/A</v>
@@ -23054,10 +23054,10 @@
         <v>1</v>
       </c>
       <c r="P19" s="243">
-        <v>4.629046311297761E-2</v>
+        <v>4.3623533650219121E-2</v>
       </c>
       <c r="Q19" s="243">
-        <v>6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R19" s="243">
         <v>0</v>
@@ -23093,25 +23093,25 @@
     </row>
     <row r="20" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="236">
-        <v>0.73411965313311145</v>
+        <v>0.74267176168050963</v>
       </c>
       <c r="B20" s="237">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="C20" s="238">
-        <v>23184.475398517086</v>
+        <v>22557.466068661157</v>
       </c>
       <c r="D20" s="238">
         <v>1000000</v>
       </c>
       <c r="E20" s="237">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="F20" s="237">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="G20" s="239">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="H20" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -23120,16 +23120,16 @@
         <v>0</v>
       </c>
       <c r="J20" s="237">
-        <v>44965</v>
+        <v>44987</v>
       </c>
       <c r="K20" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L20" s="242">
-        <v>0.49589041095890413</v>
+        <v>0.50958904109589043</v>
       </c>
       <c r="M20" s="243">
-        <v>4.6753223869937771E-2</v>
+        <v>4.4265995242265176E-2</v>
       </c>
       <c r="N20" s="243" t="str">
         <v>#N/A</v>
@@ -23138,10 +23138,10 @@
         <v>1</v>
       </c>
       <c r="P20" s="243">
-        <v>4.6753223869937778E-2</v>
+        <v>4.4265995242265176E-2</v>
       </c>
       <c r="Q20" s="243">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R20" s="243">
         <v>0</v>
@@ -23177,25 +23177,25 @@
     </row>
     <row r="21" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="236">
-        <v>0.71794182972811249</v>
+        <v>0.72750438324808642</v>
       </c>
       <c r="B21" s="237">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="C21" s="238">
-        <v>23987.60979353853</v>
+        <v>22472.158674865073</v>
       </c>
       <c r="D21" s="238">
         <v>1000000</v>
       </c>
       <c r="E21" s="237">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="F21" s="237">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="G21" s="239">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H21" s="240" t="str">
         <v>BBSW6M Actual/365 (Fixed)</v>
@@ -23204,16 +23204,16 @@
         <v>0</v>
       </c>
       <c r="J21" s="237">
-        <v>45146</v>
+        <v>45173</v>
       </c>
       <c r="K21" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
       </c>
       <c r="L21" s="242">
-        <v>0.50410958904109593</v>
+        <v>0.49863013698630138</v>
       </c>
       <c r="M21" s="243">
-        <v>4.7584117253486755E-2</v>
+        <v>4.5067790749042588E-2</v>
       </c>
       <c r="N21" s="243" t="str">
         <v>#N/A</v>
@@ -23222,10 +23222,10 @@
         <v>1</v>
       </c>
       <c r="P21" s="243">
-        <v>4.7584117253486762E-2</v>
+        <v>4.5067790749042588E-2</v>
       </c>
       <c r="Q21" s="243">
-        <v>-6.9388939039072284E-18</v>
+        <v>0</v>
       </c>
       <c r="R21" s="243">
         <v>0</v>
@@ -23261,22 +23261,22 @@
     </row>
     <row r="22" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="236">
-        <v>0.70208555969117814</v>
+        <v>0.71237079582453067</v>
       </c>
       <c r="B22" s="237">
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="C22" s="238">
-        <v>24089.918220958407</v>
+        <v>22841.713437143029</v>
       </c>
       <c r="D22" s="238">
         <v>1000000</v>
       </c>
       <c r="E22" s="237">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="F22" s="237">
-        <v>45512</v>
+        <v>45537</v>
       </c>
       <c r="G22" s="239">
         <v>182</v>
@@ -23288,7 +23288,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="237">
-        <v>45330</v>
+        <v>45355</v>
       </c>
       <c r="K22" s="239" t="str">
         <v>Actual/365 (Fixed)</v>
@@ -23297,7 +23297,7 @@
         <v>0.49863013698630138</v>
       </c>
       <c r="M22" s="243">
-        <v>4.8312198629944056E-2</v>
+        <v>4.5808930794270362E-2</v>
       </c>
       <c r="N22" s="243" t="str">
         <v>#N/A</v>
@@ -23306,7 +23306,7 @@
         <v>1</v>
       </c>
       <c r="P22" s="243">
-        <v>4.8312198629944056E-2</v>
+        <v>4.5808930794270362E-2</v>
       </c>
       <c r="Q22" s="243">
         <v>0</v>

</xml_diff>